<commit_message>
MF attention and MF_no_reinit fit result
</commit_message>
<xml_diff>
--- a/data_analysis/fit_result.xlsx
+++ b/data_analysis/fit_result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Developer/Python/RLpsy/data_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zac/Documents/RLpsy/data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{701286B9-4C58-234B-BACF-75896DC7E300}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9D7B4272-1E3A-6F4A-90F3-14100F4B9578}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34080" yWindow="-4780" windowWidth="24820" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14160" yWindow="12600" windowWidth="44260" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MF_fit_result" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="27">
   <si>
     <t>participant</t>
   </si>
@@ -90,12 +90,24 @@
   <si>
     <t>Gated_MF</t>
   </si>
+  <si>
+    <t>alpha_attention</t>
+  </si>
+  <si>
+    <t>forget_attention</t>
+  </si>
+  <si>
+    <t>MF_attention</t>
+  </si>
+  <si>
+    <t>MF_no_reinit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -940,18 +952,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CE40"/>
+  <dimension ref="A1:CW40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U21" workbookViewId="0">
-      <selection activeCell="AF43" sqref="AF43"/>
+    <sheetView tabSelected="1" topLeftCell="O13" workbookViewId="0">
+      <selection activeCell="AH3" sqref="AH3:AH38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83">
+    <row r="1" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -976,8 +988,14 @@
       <c r="BX1" t="s">
         <v>21</v>
       </c>
+      <c r="CG1" t="s">
+        <v>25</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:83">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1065,6 +1083,12 @@
       <c r="AF2" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="AG2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="AI2" t="s">
         <v>0</v>
       </c>
@@ -1191,8 +1215,56 @@
       <c r="CE2" t="s">
         <v>11</v>
       </c>
+      <c r="CG2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>1</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>2</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>4</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>5</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>23</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>24</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>11</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>1</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>2</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>4</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>5</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:83">
+    <row r="3" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1266,27 +1338,35 @@
         <v>965.06855509955335</v>
       </c>
       <c r="AA3">
-        <f>IF(AND(G3&lt;N3, G3&lt;Y3, G3&lt;AQ3,G3&lt;BC3,G3&lt;CE3),1,0)</f>
+        <f>IF(AND(G3&lt;N3, G3&lt;Y3, G3&lt;AQ3,G3&lt;BC3,G3&lt;CE3, G3&lt;CO3, G3&lt;CW3),1,0)</f>
         <v>0</v>
       </c>
       <c r="AB3">
-        <f>IF(AND(G3&gt;N3, N3&lt;Y3, N3&lt;AQ3, N3&lt;BC3, N3&lt;CE3),1,0)</f>
+        <f>IF(AND(G3&gt;N3, N3&lt;Y3, N3&lt;AQ3, N3&lt;BC3, N3&lt;CE3, N3&lt;CO3, N3&lt;CW3),1,0)</f>
         <v>0</v>
       </c>
       <c r="AC3">
-        <f>IF(AND(G3&gt;Y3, N3&gt;Y3, Y3&lt;AQ3,Y3&lt;BC3, Y3&lt;CE3),1,0)</f>
+        <f>IF(AND(G3&gt;Y3, N3&gt;Y3, Y3&lt;AQ3,Y3&lt;BC3, Y3&lt;CE3, Y3&lt;CO3, Y3&lt;CW3),1,0)</f>
         <v>0</v>
       </c>
       <c r="AD3">
-        <f>IF(AND(G3&gt;AQ3, N3&gt;AQ3, Y3&gt;AQ3,AQ3&lt;BC3,AQ3&lt;CE3),1,0)</f>
+        <f>IF(AND(G3&gt;AQ3, N3&gt;AQ3, Y3&gt;AQ3,AQ3&lt;BC3,AQ3&lt;CE3, AQ3&lt;CO3, AQ3&lt;CW3),1,0)</f>
         <v>0</v>
       </c>
       <c r="AE3">
-        <f>IF(AND(G3&gt;BC3, Y3&gt;BC3, G3&gt;BC3,AQ3&gt;BC3,BC3&lt;CE3),1,0)</f>
+        <f>IF(AND(G3&gt;BC3, Y3&gt;BC3, G3&gt;BC3,AQ3&gt;BC3,BC3&lt;CE3, BC3&lt;CO3, BC3&lt;CW3),1,0)</f>
         <v>1</v>
       </c>
       <c r="AF3">
-        <f>IF(AND(G3&gt;CE3, Y3&gt;CE3, G3&gt;CE3,AQ3&gt;CE3,BC3&gt;CE3),1,0)</f>
+        <f>IF(AND(G3&gt;CE3, Y3&gt;CE3, N3&gt;CE3,AQ3&gt;CE3,BC3&gt;CE3, CE3&lt;CO3, CE3&lt;CW3),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <f>IF(AND(G3&gt;CO3, Y3&gt;CO3, N3&gt;CO3,AQ3&gt;CO3,BC3&gt;CO3, CE3&gt;CO3, CO3&lt;CW3),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <f>IF(AND(G3&gt;CW3, Y3&gt;CW3, N3&gt;CW3,AQ3&gt;CW3,BC3&gt;CW3, CE3&gt;CW3, CO3&gt;CW3),1,0)</f>
         <v>0</v>
       </c>
       <c r="AI3">
@@ -1428,8 +1508,58 @@
         <f>BY3+2*5*(144/(144-5-1))</f>
         <v>964.11120680939666</v>
       </c>
+      <c r="CG3">
+        <v>0</v>
+      </c>
+      <c r="CH3">
+        <v>948.51045369062399</v>
+      </c>
+      <c r="CI3">
+        <v>3.8915330706178003E-2</v>
+      </c>
+      <c r="CJ3">
+        <v>0.61371789523851705</v>
+      </c>
+      <c r="CK3">
+        <v>1</v>
+      </c>
+      <c r="CL3">
+        <v>2.6934781151845598E-3</v>
+      </c>
+      <c r="CM3">
+        <v>1.2043779259776E-2</v>
+      </c>
+      <c r="CN3">
+        <v>0</v>
+      </c>
+      <c r="CO3">
+        <f>CH3+2*6*(144/(144-6-1))</f>
+        <v>961.12359237675537</v>
+      </c>
+      <c r="CQ3">
+        <v>0</v>
+      </c>
+      <c r="CR3">
+        <v>1062.12196783686</v>
+      </c>
+      <c r="CS3">
+        <v>0.11171883074804601</v>
+      </c>
+      <c r="CT3">
+        <v>0.210722038225545</v>
+      </c>
+      <c r="CU3">
+        <v>1</v>
+      </c>
+      <c r="CV3">
+        <v>4.2370595591307002E-4</v>
+      </c>
+      <c r="CW3">
+        <f>CR3+2*4*(144/(144-4-1))</f>
+        <v>1070.4097376210327</v>
+      </c>
     </row>
-    <row r="4" spans="1:83">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1503,27 +1633,35 @@
         <v>1646.0169070331015</v>
       </c>
       <c r="AA4">
-        <f t="shared" ref="AA4:AA38" si="4">IF(AND(G4&lt;N4, G4&lt;Y4, G4&lt;AQ4,G4&lt;BC4,G4&lt;CE4),1,0)</f>
+        <f t="shared" ref="AA4:AA38" si="4">IF(AND(G4&lt;N4, G4&lt;Y4, G4&lt;AQ4,G4&lt;BC4,G4&lt;CE4, G4&lt;CO4, G4&lt;CW4),1,0)</f>
         <v>1</v>
       </c>
       <c r="AB4">
-        <f t="shared" ref="AB4:AB38" si="5">IF(AND(G4&gt;N4, N4&lt;Y4, N4&lt;AQ4, N4&lt;BC4, N4&lt;CE4),1,0)</f>
+        <f t="shared" ref="AB4:AB38" si="5">IF(AND(G4&gt;N4, N4&lt;Y4, N4&lt;AQ4, N4&lt;BC4, N4&lt;CE4, N4&lt;CO4, N4&lt;CW4),1,0)</f>
         <v>0</v>
       </c>
       <c r="AC4">
-        <f t="shared" ref="AC4:AC38" si="6">IF(AND(G4&gt;Y4, N4&gt;Y4, Y4&lt;AQ4,Y4&lt;BC4, Y4&lt;CE4),1,0)</f>
+        <f t="shared" ref="AC4:AC37" si="6">IF(AND(G4&gt;Y4, N4&gt;Y4, Y4&lt;AQ4,Y4&lt;BC4, Y4&lt;CE4, Y4&lt;CO4, Y4&lt;CW4),1,0)</f>
         <v>0</v>
       </c>
       <c r="AD4">
-        <f t="shared" ref="AD4:AD38" si="7">IF(AND(G4&gt;AQ4, N4&gt;AQ4, Y4&gt;AQ4,AQ4&lt;BC4,AQ4&lt;CE4),1,0)</f>
+        <f t="shared" ref="AD4:AD38" si="7">IF(AND(G4&gt;AQ4, N4&gt;AQ4, Y4&gt;AQ4,AQ4&lt;BC4,AQ4&lt;CE4, AQ4&lt;CO4, AQ4&lt;CW4),1,0)</f>
         <v>0</v>
       </c>
       <c r="AE4">
-        <f t="shared" ref="AE4:AE38" si="8">IF(AND(G4&gt;BC4, Y4&gt;BC4, G4&gt;BC4,AQ4&gt;BC4,BC4&lt;CE4),1,0)</f>
+        <f t="shared" ref="AE4:AE38" si="8">IF(AND(G4&gt;BC4, Y4&gt;BC4, G4&gt;BC4,AQ4&gt;BC4,BC4&lt;CE4, BC4&lt;CO4, BC4&lt;CW4),1,0)</f>
         <v>0</v>
       </c>
       <c r="AF4">
-        <f t="shared" ref="AF4:AF38" si="9">IF(AND(G4&gt;CE4, Y4&gt;CE4, G4&gt;CE4,AQ4&gt;CE4,BC4&gt;CE4),1,0)</f>
+        <f t="shared" ref="AF4:AF38" si="9">IF(AND(G4&gt;CE4, Y4&gt;CE4, N4&gt;CE4,AQ4&gt;CE4,BC4&gt;CE4, CE4&lt;CO4, CE4&lt;CW4),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <f t="shared" ref="AG4:AG38" si="10">IF(AND(G4&gt;CO4, Y4&gt;CO4, N4&gt;CO4,AQ4&gt;CO4,BC4&gt;CO4, CE4&gt;CO4, CO4&lt;CW4),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <f t="shared" ref="AH4:AH38" si="11">IF(AND(G4&gt;CW4, Y4&gt;CW4, N4&gt;CW4,AQ4&gt;CW4,BC4&gt;CW4, CE4&gt;CW4, CO4&gt;CW4),1,0)</f>
         <v>0</v>
       </c>
       <c r="AI4">
@@ -1551,7 +1689,7 @@
         <v>1.6655015192281501E-3</v>
       </c>
       <c r="AQ4">
-        <f t="shared" ref="AQ4:AQ38" si="10">AJ4+2*6*(144/(144-6-1))</f>
+        <f t="shared" ref="AQ4:AQ38" si="12">AJ4+2*6*(144/(144-6-1))</f>
         <v>1697.8250933813413</v>
       </c>
       <c r="AS4">
@@ -1607,15 +1745,15 @@
         <v>2.5923689999999999E-2</v>
       </c>
       <c r="BL4">
-        <f t="shared" ref="BL4:BL38" si="11">BG4+2*3*(144/(144-3-1))</f>
+        <f t="shared" ref="BL4:BL38" si="13">BG4+2*3*(144/(144-3-1))</f>
         <v>1640.0163385714286</v>
       </c>
       <c r="BN4">
-        <f t="shared" ref="BN4:BN38" si="12">IF(G4&lt;BL4,1,0)</f>
+        <f t="shared" ref="BN4:BN38" si="14">IF(G4&lt;BL4,1,0)</f>
         <v>0</v>
       </c>
       <c r="BO4" s="3">
-        <f t="shared" ref="BO4:BO38" si="13">IF(G4&lt;BV4,1,0)</f>
+        <f t="shared" ref="BO4:BO38" si="15">IF(G4&lt;BV4,1,0)</f>
         <v>1</v>
       </c>
       <c r="BP4" s="3">
@@ -1637,7 +1775,7 @@
         <v>0</v>
       </c>
       <c r="BV4">
-        <f t="shared" ref="BV4:BV38" si="14">BQ4+2*4*(144/(144-4-1))</f>
+        <f t="shared" ref="BV4:BV38" si="16">BQ4+2*4*(144/(144-4-1))</f>
         <v>1644.6597197841727</v>
       </c>
       <c r="BX4">
@@ -1662,11 +1800,61 @@
         <v>0.163089418570672</v>
       </c>
       <c r="CE4">
-        <f t="shared" ref="CE4:CE38" si="15">BY4+2*5*(144/(144-5-1))</f>
+        <f t="shared" ref="CE4:CE38" si="17">BY4+2*5*(144/(144-5-1))</f>
         <v>1643.9568758352157</v>
       </c>
+      <c r="CG4">
+        <v>1</v>
+      </c>
+      <c r="CH4">
+        <v>1635.34725024046</v>
+      </c>
+      <c r="CI4">
+        <v>1.3543457546678401E-2</v>
+      </c>
+      <c r="CJ4">
+        <v>0.16495681426310399</v>
+      </c>
+      <c r="CK4">
+        <v>1</v>
+      </c>
+      <c r="CL4" s="1">
+        <v>9.5044858105273504E-5</v>
+      </c>
+      <c r="CM4">
+        <v>0.96517727550497001</v>
+      </c>
+      <c r="CN4">
+        <v>1.9502928637971199E-3</v>
+      </c>
+      <c r="CO4">
+        <f t="shared" ref="CO4:CO38" si="18">CH4+2*6*(144/(144-6-1))</f>
+        <v>1647.9603889265913</v>
+      </c>
+      <c r="CQ4">
+        <v>1</v>
+      </c>
+      <c r="CR4">
+        <v>1660.4830819869601</v>
+      </c>
+      <c r="CS4">
+        <v>0.15602604724191699</v>
+      </c>
+      <c r="CT4">
+        <v>0.19303521304885099</v>
+      </c>
+      <c r="CU4">
+        <v>1</v>
+      </c>
+      <c r="CV4">
+        <v>2.1609632546999501E-3</v>
+      </c>
+      <c r="CW4">
+        <f t="shared" ref="CW4:CW38" si="19">CR4+2*4*(144/(144-4-1))</f>
+        <v>1668.7708517711328</v>
+      </c>
     </row>
-    <row r="5" spans="1:83">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1741,7 +1929,7 @@
       </c>
       <c r="AA5">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB5">
         <f t="shared" si="5"/>
@@ -1763,6 +1951,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG5">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
       <c r="AI5">
         <v>2</v>
       </c>
@@ -1788,7 +1984,7 @@
         <v>0</v>
       </c>
       <c r="AQ5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1650.5855718645314</v>
       </c>
       <c r="AS5">
@@ -1844,15 +2040,15 @@
         <v>1.0178380000000001E-2</v>
       </c>
       <c r="BL5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1491.4057285714287</v>
       </c>
       <c r="BN5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO5" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP5" s="3">
@@ -1874,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="BV5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1553.5259397841728</v>
       </c>
       <c r="BX5">
@@ -1899,11 +2095,61 @@
         <v>0.104983228273306</v>
       </c>
       <c r="CE5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1493.0355464825057</v>
       </c>
+      <c r="CG5">
+        <v>2</v>
+      </c>
+      <c r="CH5">
+        <v>1494.5970165056499</v>
+      </c>
+      <c r="CI5">
+        <v>2.0496989743865001E-2</v>
+      </c>
+      <c r="CJ5">
+        <v>0.24548109779379601</v>
+      </c>
+      <c r="CK5">
+        <v>1</v>
+      </c>
+      <c r="CL5">
+        <v>7.2306813513348003E-4</v>
+      </c>
+      <c r="CM5">
+        <v>0.29469265805834999</v>
+      </c>
+      <c r="CN5">
+        <v>0</v>
+      </c>
+      <c r="CO5">
+        <f t="shared" si="18"/>
+        <v>1507.2101551917813</v>
+      </c>
+      <c r="CQ5">
+        <v>2</v>
+      </c>
+      <c r="CR5">
+        <v>1433.1553808833301</v>
+      </c>
+      <c r="CS5">
+        <v>5.01557527688445E-2</v>
+      </c>
+      <c r="CT5">
+        <v>0.482590284554898</v>
+      </c>
+      <c r="CU5">
+        <v>1</v>
+      </c>
+      <c r="CV5">
+        <v>0</v>
+      </c>
+      <c r="CW5">
+        <f t="shared" si="19"/>
+        <v>1441.4431506675028</v>
+      </c>
     </row>
-    <row r="6" spans="1:83">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2000,6 +2246,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI6">
         <v>3</v>
       </c>
@@ -2025,7 +2279,7 @@
         <v>2.1679496888962098E-3</v>
       </c>
       <c r="AQ6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>763.82061215463534</v>
       </c>
       <c r="AS6">
@@ -2081,15 +2335,15 @@
         <v>4.1014559999999999E-2</v>
       </c>
       <c r="BL6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>706.45906957142859</v>
       </c>
       <c r="BN6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO6" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP6" s="3">
@@ -2111,7 +2365,7 @@
         <v>3.2482789999999997E-2</v>
       </c>
       <c r="BV6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>663.36181478417257</v>
       </c>
       <c r="BX6">
@@ -2136,11 +2390,61 @@
         <v>0.93218980480047298</v>
       </c>
       <c r="CE6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>660.12272272447967</v>
       </c>
+      <c r="CG6">
+        <v>3</v>
+      </c>
+      <c r="CH6">
+        <v>648.17146157898298</v>
+      </c>
+      <c r="CI6">
+        <v>2.8629892594353099E-2</v>
+      </c>
+      <c r="CJ6">
+        <v>0.43562658565628898</v>
+      </c>
+      <c r="CK6">
+        <v>1</v>
+      </c>
+      <c r="CL6">
+        <v>3.4945006712880797E-2</v>
+      </c>
+      <c r="CM6">
+        <v>0.20176045508447599</v>
+      </c>
+      <c r="CN6">
+        <v>4.36666381297915E-4</v>
+      </c>
+      <c r="CO6">
+        <f t="shared" si="18"/>
+        <v>660.78460026511436</v>
+      </c>
+      <c r="CQ6">
+        <v>3</v>
+      </c>
+      <c r="CR6">
+        <v>673.51755158424101</v>
+      </c>
+      <c r="CS6">
+        <v>0.40386790011090701</v>
+      </c>
+      <c r="CT6">
+        <v>0.30002699392996401</v>
+      </c>
+      <c r="CU6">
+        <v>1</v>
+      </c>
+      <c r="CV6">
+        <v>2.8378020614883901E-2</v>
+      </c>
+      <c r="CW6">
+        <f t="shared" si="19"/>
+        <v>681.80532136841362</v>
+      </c>
     </row>
-    <row r="7" spans="1:83">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2215,7 +2519,7 @@
       </c>
       <c r="AA7">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB7">
         <f t="shared" si="5"/>
@@ -2237,6 +2541,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG7">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
       <c r="AI7">
         <v>4</v>
       </c>
@@ -2262,7 +2574,7 @@
         <v>0.05</v>
       </c>
       <c r="AQ7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1939.9785948647714</v>
       </c>
       <c r="AS7">
@@ -2318,15 +2630,15 @@
         <v>8.6045500000000007E-3</v>
       </c>
       <c r="BL7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1931.5904485714286</v>
       </c>
       <c r="BN7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BO7" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BP7" s="3">
@@ -2348,7 +2660,7 @@
         <v>3.1319710000000001E-2</v>
       </c>
       <c r="BV7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1934.8961497841726</v>
       </c>
       <c r="BX7">
@@ -2373,11 +2685,61 @@
         <v>0.21153233448893599</v>
       </c>
       <c r="CE7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1937.1650414868157</v>
       </c>
+      <c r="CG7">
+        <v>4</v>
+      </c>
+      <c r="CH7">
+        <v>1923.3650736054201</v>
+      </c>
+      <c r="CI7">
+        <v>7.9874754835646294E-2</v>
+      </c>
+      <c r="CJ7">
+        <v>3.6145101110742699E-2</v>
+      </c>
+      <c r="CK7">
+        <v>0.99981802729856695</v>
+      </c>
+      <c r="CL7">
+        <v>1.20055240746218E-3</v>
+      </c>
+      <c r="CM7">
+        <v>1</v>
+      </c>
+      <c r="CN7">
+        <v>5.7307374299933799E-3</v>
+      </c>
+      <c r="CO7">
+        <f t="shared" si="18"/>
+        <v>1935.9782122915515</v>
+      </c>
+      <c r="CQ7">
+        <v>4</v>
+      </c>
+      <c r="CR7">
+        <v>1918.1807700028401</v>
+      </c>
+      <c r="CS7">
+        <v>9.2768577157855095E-2</v>
+      </c>
+      <c r="CT7">
+        <v>0.19119220578099699</v>
+      </c>
+      <c r="CU7">
+        <v>1</v>
+      </c>
+      <c r="CV7">
+        <v>0</v>
+      </c>
+      <c r="CW7">
+        <f t="shared" si="19"/>
+        <v>1926.4685397870128</v>
+      </c>
     </row>
-    <row r="8" spans="1:83">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2474,6 +2836,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI8">
         <v>5</v>
       </c>
@@ -2499,7 +2869,7 @@
         <v>1.22489636740352E-3</v>
       </c>
       <c r="AQ8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>881.6641827841064</v>
       </c>
       <c r="AS8">
@@ -2555,15 +2925,15 @@
         <v>1.131222E-2</v>
       </c>
       <c r="BL8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>809.7866035714286</v>
       </c>
       <c r="BN8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO8" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP8" s="3">
@@ -2585,7 +2955,7 @@
         <v>2.3553439999999998E-2</v>
       </c>
       <c r="BV8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>808.78854978417257</v>
       </c>
       <c r="BX8">
@@ -2610,11 +2980,61 @@
         <v>0.94109653542774496</v>
       </c>
       <c r="CE8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>789.85269536105568</v>
       </c>
+      <c r="CG8">
+        <v>5</v>
+      </c>
+      <c r="CH8">
+        <v>788.81392239227898</v>
+      </c>
+      <c r="CI8">
+        <v>2.5019400000391399E-2</v>
+      </c>
+      <c r="CJ8">
+        <v>0.30163260384053597</v>
+      </c>
+      <c r="CK8">
+        <v>1</v>
+      </c>
+      <c r="CL8">
+        <v>8.9595282752376205E-3</v>
+      </c>
+      <c r="CM8">
+        <v>0.69716875170043302</v>
+      </c>
+      <c r="CN8">
+        <v>0</v>
+      </c>
+      <c r="CO8">
+        <f t="shared" si="18"/>
+        <v>801.42706107841036</v>
+      </c>
+      <c r="CQ8">
+        <v>5</v>
+      </c>
+      <c r="CR8">
+        <v>856.33549233861697</v>
+      </c>
+      <c r="CS8">
+        <v>0.41819778829693599</v>
+      </c>
+      <c r="CT8">
+        <v>0.239254725207873</v>
+      </c>
+      <c r="CU8">
+        <v>1</v>
+      </c>
+      <c r="CV8">
+        <v>1.9461298932469801E-2</v>
+      </c>
+      <c r="CW8">
+        <f t="shared" si="19"/>
+        <v>864.62326212278958</v>
+      </c>
     </row>
-    <row r="9" spans="1:83">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2689,7 +3109,7 @@
       </c>
       <c r="AA9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB9">
         <f t="shared" si="5"/>
@@ -2711,6 +3131,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG9">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI9">
         <v>6</v>
       </c>
@@ -2736,7 +3164,7 @@
         <v>2.9544906051947798E-4</v>
       </c>
       <c r="AQ9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1140.1691452392813</v>
       </c>
       <c r="AS9">
@@ -2792,15 +3220,15 @@
         <v>2.9430699999999999E-3</v>
       </c>
       <c r="BL9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1059.8757885714285</v>
       </c>
       <c r="BN9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BO9" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP9" s="3">
@@ -2822,7 +3250,7 @@
         <v>1.2952700000000001E-3</v>
       </c>
       <c r="BV9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1070.7229997841728</v>
       </c>
       <c r="BX9">
@@ -2847,11 +3275,61 @@
         <v>0.24214375732406801</v>
       </c>
       <c r="CE9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1062.4484125601057</v>
       </c>
+      <c r="CG9">
+        <v>6</v>
+      </c>
+      <c r="CH9">
+        <v>1045.2269719532001</v>
+      </c>
+      <c r="CI9">
+        <v>1.5659712809123299E-2</v>
+      </c>
+      <c r="CJ9">
+        <v>0.22480743457302199</v>
+      </c>
+      <c r="CK9">
+        <v>1</v>
+      </c>
+      <c r="CL9">
+        <v>1.14099106972547E-3</v>
+      </c>
+      <c r="CM9">
+        <v>0.320237075842423</v>
+      </c>
+      <c r="CN9">
+        <v>0</v>
+      </c>
+      <c r="CO9">
+        <f t="shared" si="18"/>
+        <v>1057.8401106393314</v>
+      </c>
+      <c r="CQ9">
+        <v>6</v>
+      </c>
+      <c r="CR9">
+        <v>1140.2567847873499</v>
+      </c>
+      <c r="CS9">
+        <v>6.7232119672754595E-2</v>
+      </c>
+      <c r="CT9">
+        <v>0.17648542827740599</v>
+      </c>
+      <c r="CU9">
+        <v>1</v>
+      </c>
+      <c r="CV9">
+        <v>0</v>
+      </c>
+      <c r="CW9">
+        <f t="shared" si="19"/>
+        <v>1148.5445545715227</v>
+      </c>
     </row>
-    <row r="10" spans="1:83">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2948,6 +3426,14 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
+      <c r="AG10">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI10">
         <v>7</v>
       </c>
@@ -2973,7 +3459,7 @@
         <v>1.60436627189665E-4</v>
       </c>
       <c r="AQ10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1475.5884957285714</v>
       </c>
       <c r="AS10">
@@ -3029,15 +3515,15 @@
         <v>2.8443909999999999E-2</v>
       </c>
       <c r="BL10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1273.2109585714286</v>
       </c>
       <c r="BN10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO10" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP10" s="3">
@@ -3059,7 +3545,7 @@
         <v>8.8772499999999997E-3</v>
       </c>
       <c r="BV10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1295.1120497841728</v>
       </c>
       <c r="BX10">
@@ -3084,11 +3570,61 @@
         <v>0.429163392759773</v>
       </c>
       <c r="CE10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1216.1098920463057</v>
       </c>
+      <c r="CG10">
+        <v>7</v>
+      </c>
+      <c r="CH10">
+        <v>1220.00105430435</v>
+      </c>
+      <c r="CI10">
+        <v>3.9866628676283801E-2</v>
+      </c>
+      <c r="CJ10">
+        <v>0.29830240084623399</v>
+      </c>
+      <c r="CK10">
+        <v>1</v>
+      </c>
+      <c r="CL10">
+        <v>5.9650327839560601E-3</v>
+      </c>
+      <c r="CM10">
+        <v>0.61219857696830604</v>
+      </c>
+      <c r="CN10">
+        <v>0</v>
+      </c>
+      <c r="CO10">
+        <f t="shared" si="18"/>
+        <v>1232.6141929904813</v>
+      </c>
+      <c r="CQ10">
+        <v>7</v>
+      </c>
+      <c r="CR10">
+        <v>1235.06537332835</v>
+      </c>
+      <c r="CS10">
+        <v>0.48689077812209203</v>
+      </c>
+      <c r="CT10">
+        <v>0.29248807524527698</v>
+      </c>
+      <c r="CU10">
+        <v>1</v>
+      </c>
+      <c r="CV10">
+        <v>8.4521911175785593E-3</v>
+      </c>
+      <c r="CW10">
+        <f t="shared" si="19"/>
+        <v>1243.3531431125227</v>
+      </c>
     </row>
-    <row r="11" spans="1:83">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -3179,12 +3715,20 @@
       </c>
       <c r="AE11">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF11">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI11">
         <v>8</v>
       </c>
@@ -3210,7 +3754,7 @@
         <v>0</v>
       </c>
       <c r="AQ11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1297.6462958316713</v>
       </c>
       <c r="AS11">
@@ -3266,15 +3810,15 @@
         <v>2.5773330000000001E-2</v>
       </c>
       <c r="BL11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>940.45210057142856</v>
       </c>
       <c r="BN11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO11" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP11" s="3">
@@ -3296,7 +3840,7 @@
         <v>0</v>
       </c>
       <c r="BV11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>982.14851978417266</v>
       </c>
       <c r="BX11">
@@ -3321,11 +3865,61 @@
         <v>1.77051357177349E-2</v>
       </c>
       <c r="CE11">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>938.29023365442458</v>
       </c>
+      <c r="CG11">
+        <v>8</v>
+      </c>
+      <c r="CH11">
+        <v>921.48093901155903</v>
+      </c>
+      <c r="CI11">
+        <v>3.2654036668424202E-2</v>
+      </c>
+      <c r="CJ11">
+        <v>0.29078208985172999</v>
+      </c>
+      <c r="CK11">
+        <v>1</v>
+      </c>
+      <c r="CL11">
+        <v>1.74823100310799E-3</v>
+      </c>
+      <c r="CM11">
+        <v>1</v>
+      </c>
+      <c r="CN11">
+        <v>0</v>
+      </c>
+      <c r="CO11">
+        <f t="shared" si="18"/>
+        <v>934.09407769769041</v>
+      </c>
+      <c r="CQ11">
+        <v>8</v>
+      </c>
+      <c r="CR11">
+        <v>948.692356417209</v>
+      </c>
+      <c r="CS11">
+        <v>7.8016923026755697E-2</v>
+      </c>
+      <c r="CT11">
+        <v>0.482590157334916</v>
+      </c>
+      <c r="CU11">
+        <v>1</v>
+      </c>
+      <c r="CV11" s="1">
+        <v>8.8030855769607598E-5</v>
+      </c>
+      <c r="CW11">
+        <f t="shared" si="19"/>
+        <v>956.98012620138161</v>
+      </c>
     </row>
-    <row r="12" spans="1:83">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -3422,6 +4016,14 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
+      <c r="AG12">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI12">
         <v>9</v>
       </c>
@@ -3447,7 +4049,7 @@
         <v>2.7294819753696702E-3</v>
       </c>
       <c r="AQ12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>688.89376505465736</v>
       </c>
       <c r="AS12">
@@ -3503,15 +4105,15 @@
         <v>1.1050829999999999E-2</v>
       </c>
       <c r="BL12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>420.81056757142858</v>
       </c>
       <c r="BN12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO12" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP12" s="3">
@@ -3533,7 +4135,7 @@
         <v>1.2417910000000001E-2</v>
       </c>
       <c r="BV12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>403.69696278417268</v>
       </c>
       <c r="BX12">
@@ -3558,11 +4160,61 @@
         <v>1.46342798154029E-2</v>
       </c>
       <c r="CE12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>378.31219255711062</v>
       </c>
+      <c r="CG12">
+        <v>9</v>
+      </c>
+      <c r="CH12">
+        <v>383.79313286458199</v>
+      </c>
+      <c r="CI12">
+        <v>3.1408564879711103E-2</v>
+      </c>
+      <c r="CJ12">
+        <v>0.40904391050377398</v>
+      </c>
+      <c r="CK12">
+        <v>1</v>
+      </c>
+      <c r="CL12">
+        <v>8.2773107594032794E-3</v>
+      </c>
+      <c r="CM12">
+        <v>1</v>
+      </c>
+      <c r="CN12">
+        <v>0</v>
+      </c>
+      <c r="CO12">
+        <f t="shared" si="18"/>
+        <v>396.40627155071337</v>
+      </c>
+      <c r="CQ12">
+        <v>9</v>
+      </c>
+      <c r="CR12">
+        <v>510.70510869050503</v>
+      </c>
+      <c r="CS12">
+        <v>0.67967555385215705</v>
+      </c>
+      <c r="CT12">
+        <v>0.28652781649977999</v>
+      </c>
+      <c r="CU12">
+        <v>1</v>
+      </c>
+      <c r="CV12">
+        <v>1.6372946970727199E-2</v>
+      </c>
+      <c r="CW12">
+        <f t="shared" si="19"/>
+        <v>518.9928784746777</v>
+      </c>
     </row>
-    <row r="13" spans="1:83">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -3659,6 +4311,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH13">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI13">
         <v>10</v>
       </c>
@@ -3684,7 +4344,7 @@
         <v>0</v>
       </c>
       <c r="AQ13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1074.0780479108314</v>
       </c>
       <c r="AS13">
@@ -3740,15 +4400,15 @@
         <v>1.599215E-2</v>
       </c>
       <c r="BL13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>967.90764457142859</v>
       </c>
       <c r="BN13">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO13" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP13" s="3">
@@ -3770,7 +4430,7 @@
         <v>4.2341000000000002E-3</v>
       </c>
       <c r="BV13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>957.64559278417266</v>
       </c>
       <c r="BX13">
@@ -3795,11 +4455,61 @@
         <v>0.71842636833682005</v>
       </c>
       <c r="CE13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>949.31331974965963</v>
       </c>
+      <c r="CG13">
+        <v>10</v>
+      </c>
+      <c r="CH13">
+        <v>933.75653020790799</v>
+      </c>
+      <c r="CI13">
+        <v>2.54070464572499E-2</v>
+      </c>
+      <c r="CJ13">
+        <v>0.276736408280982</v>
+      </c>
+      <c r="CK13">
+        <v>1</v>
+      </c>
+      <c r="CL13">
+        <v>5.4381711406875002E-3</v>
+      </c>
+      <c r="CM13">
+        <v>0.97542871234347495</v>
+      </c>
+      <c r="CN13">
+        <v>0</v>
+      </c>
+      <c r="CO13">
+        <f t="shared" si="18"/>
+        <v>946.36966889403936</v>
+      </c>
+      <c r="CQ13">
+        <v>10</v>
+      </c>
+      <c r="CR13">
+        <v>1030.4085923927801</v>
+      </c>
+      <c r="CS13">
+        <v>8.0276612176464895E-2</v>
+      </c>
+      <c r="CT13">
+        <v>0.32444794607382299</v>
+      </c>
+      <c r="CU13">
+        <v>1</v>
+      </c>
+      <c r="CV13">
+        <v>0</v>
+      </c>
+      <c r="CW13">
+        <f t="shared" si="19"/>
+        <v>1038.6963621769528</v>
+      </c>
     </row>
-    <row r="14" spans="1:83">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -3896,6 +4606,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI14">
         <v>11</v>
       </c>
@@ -3921,7 +4639,7 @@
         <v>0</v>
       </c>
       <c r="AQ14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>957.89898073113943</v>
       </c>
       <c r="AS14">
@@ -3977,15 +4695,15 @@
         <v>3.8986229999999997E-2</v>
       </c>
       <c r="BL14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>874.32833757142862</v>
       </c>
       <c r="BN14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO14" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP14" s="3">
@@ -4007,7 +4725,7 @@
         <v>1.7991800000000001E-3</v>
       </c>
       <c r="BV14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>877.73671878417258</v>
       </c>
       <c r="BX14">
@@ -4032,11 +4750,61 @@
         <v>0.39313120269083301</v>
       </c>
       <c r="CE14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>871.36455500062766</v>
       </c>
+      <c r="CG14">
+        <v>11</v>
+      </c>
+      <c r="CH14">
+        <v>861.04034754566703</v>
+      </c>
+      <c r="CI14">
+        <v>1.8494963590483401E-2</v>
+      </c>
+      <c r="CJ14">
+        <v>0.334839693100281</v>
+      </c>
+      <c r="CK14">
+        <v>1</v>
+      </c>
+      <c r="CL14">
+        <v>2.4809448412138799E-3</v>
+      </c>
+      <c r="CM14">
+        <v>0.22971138660778001</v>
+      </c>
+      <c r="CN14">
+        <v>0</v>
+      </c>
+      <c r="CO14">
+        <f t="shared" si="18"/>
+        <v>873.65348623179841</v>
+      </c>
+      <c r="CQ14">
+        <v>11</v>
+      </c>
+      <c r="CR14">
+        <v>918.45803326534701</v>
+      </c>
+      <c r="CS14">
+        <v>0.32155651925140699</v>
+      </c>
+      <c r="CT14">
+        <v>0.28999057068988598</v>
+      </c>
+      <c r="CU14">
+        <v>1</v>
+      </c>
+      <c r="CV14">
+        <v>1.5880435728177902E-2</v>
+      </c>
+      <c r="CW14">
+        <f t="shared" si="19"/>
+        <v>926.74580304951962</v>
+      </c>
     </row>
-    <row r="15" spans="1:83">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -4133,6 +4901,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI15">
         <v>12</v>
       </c>
@@ -4158,7 +4934,7 @@
         <v>1.7404516199019599E-3</v>
       </c>
       <c r="AQ15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>775.29128478434939</v>
       </c>
       <c r="AS15">
@@ -4214,15 +4990,15 @@
         <v>1.7486890000000001E-2</v>
       </c>
       <c r="BL15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>717.84052957142853</v>
       </c>
       <c r="BN15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO15" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP15" s="3">
@@ -4244,7 +5020,7 @@
         <v>5.1466200000000002E-3</v>
       </c>
       <c r="BV15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>707.42882678417266</v>
       </c>
       <c r="BX15">
@@ -4269,11 +5045,61 @@
         <v>0.124191244840701</v>
       </c>
       <c r="CE15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>701.59392067262365</v>
       </c>
+      <c r="CG15">
+        <v>12</v>
+      </c>
+      <c r="CH15">
+        <v>689.09298749609502</v>
+      </c>
+      <c r="CI15">
+        <v>1.6746507269712E-2</v>
+      </c>
+      <c r="CJ15">
+        <v>0.28394282968711199</v>
+      </c>
+      <c r="CK15">
+        <v>1</v>
+      </c>
+      <c r="CL15">
+        <v>4.3531140389501304E-3</v>
+      </c>
+      <c r="CM15">
+        <v>0.97721014855647004</v>
+      </c>
+      <c r="CN15">
+        <v>0</v>
+      </c>
+      <c r="CO15">
+        <f t="shared" si="18"/>
+        <v>701.7061261822264</v>
+      </c>
+      <c r="CQ15">
+        <v>12</v>
+      </c>
+      <c r="CR15">
+        <v>867.19277302957096</v>
+      </c>
+      <c r="CS15">
+        <v>0.35108474963013497</v>
+      </c>
+      <c r="CT15">
+        <v>0.157214548312409</v>
+      </c>
+      <c r="CU15">
+        <v>1</v>
+      </c>
+      <c r="CV15">
+        <v>7.2238932143918301E-3</v>
+      </c>
+      <c r="CW15">
+        <f t="shared" si="19"/>
+        <v>875.48054281374357</v>
+      </c>
     </row>
-    <row r="16" spans="1:83">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
@@ -4370,6 +5196,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI16">
         <v>13</v>
       </c>
@@ -4395,7 +5229,7 @@
         <v>1.5733377260318201E-2</v>
       </c>
       <c r="AQ16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>977.93195525001443</v>
       </c>
       <c r="AS16">
@@ -4451,15 +5285,15 @@
         <v>1.0974699999999999E-3</v>
       </c>
       <c r="BL16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>949.75762457142855</v>
       </c>
       <c r="BN16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO16" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP16" s="3">
@@ -4481,7 +5315,7 @@
         <v>4.1334799999999998E-2</v>
       </c>
       <c r="BV16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>913.68219278417257</v>
       </c>
       <c r="BX16">
@@ -4506,11 +5340,61 @@
         <v>0.68695706538742496</v>
       </c>
       <c r="CE16">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>911.01646756028561</v>
       </c>
+      <c r="CG16">
+        <v>13</v>
+      </c>
+      <c r="CH16">
+        <v>902.22344282769097</v>
+      </c>
+      <c r="CI16">
+        <v>2.9448745826485601E-2</v>
+      </c>
+      <c r="CJ16">
+        <v>0.33625213426407302</v>
+      </c>
+      <c r="CK16">
+        <v>1</v>
+      </c>
+      <c r="CL16">
+        <v>2.65451519594571E-2</v>
+      </c>
+      <c r="CM16">
+        <v>0.27285516809436899</v>
+      </c>
+      <c r="CN16">
+        <v>0</v>
+      </c>
+      <c r="CO16">
+        <f t="shared" si="18"/>
+        <v>914.83658151382235</v>
+      </c>
+      <c r="CQ16">
+        <v>13</v>
+      </c>
+      <c r="CR16">
+        <v>928.92966165113603</v>
+      </c>
+      <c r="CS16">
+        <v>0.44948891056192303</v>
+      </c>
+      <c r="CT16">
+        <v>0.26430735796983601</v>
+      </c>
+      <c r="CU16">
+        <v>1</v>
+      </c>
+      <c r="CV16">
+        <v>3.3667520088465699E-2</v>
+      </c>
+      <c r="CW16">
+        <f t="shared" si="19"/>
+        <v>937.21743143530864</v>
+      </c>
     </row>
-    <row r="17" spans="1:83">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
@@ -4607,6 +5491,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH17">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI17">
         <v>14</v>
       </c>
@@ -4632,7 +5524,7 @@
         <v>0</v>
       </c>
       <c r="AQ17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1880.2535536334715</v>
       </c>
       <c r="AS17">
@@ -4688,15 +5580,15 @@
         <v>5.5378299999999997E-3</v>
       </c>
       <c r="BL17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1608.1983685714285</v>
       </c>
       <c r="BN17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO17" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP17" s="3">
@@ -4718,7 +5610,7 @@
         <v>2.6784999999999998E-4</v>
       </c>
       <c r="BV17">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1684.6454697841727</v>
       </c>
       <c r="BX17">
@@ -4743,11 +5635,61 @@
         <v>0.98494576907271703</v>
       </c>
       <c r="CE17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1604.0811168772457</v>
       </c>
+      <c r="CG17">
+        <v>14</v>
+      </c>
+      <c r="CH17">
+        <v>1591.1071221636801</v>
+      </c>
+      <c r="CI17">
+        <v>5.0239171900815602E-2</v>
+      </c>
+      <c r="CJ17">
+        <v>0.28006468287201602</v>
+      </c>
+      <c r="CK17">
+        <v>1</v>
+      </c>
+      <c r="CL17">
+        <v>1.0417966530518201E-3</v>
+      </c>
+      <c r="CM17">
+        <v>0.48858925521928198</v>
+      </c>
+      <c r="CN17">
+        <v>3.3933558986764499E-3</v>
+      </c>
+      <c r="CO17">
+        <f t="shared" si="18"/>
+        <v>1603.7202608498114</v>
+      </c>
+      <c r="CQ17">
+        <v>14</v>
+      </c>
+      <c r="CR17">
+        <v>1621.6917878588999</v>
+      </c>
+      <c r="CS17">
+        <v>0.19740651343418</v>
+      </c>
+      <c r="CT17">
+        <v>0.39435842053620301</v>
+      </c>
+      <c r="CU17">
+        <v>1</v>
+      </c>
+      <c r="CV17">
+        <v>1.2626828963611099E-3</v>
+      </c>
+      <c r="CW17">
+        <f t="shared" si="19"/>
+        <v>1629.9795576430727</v>
+      </c>
     </row>
-    <row r="18" spans="1:83">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
@@ -4844,6 +5786,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI18">
         <v>15</v>
       </c>
@@ -4869,7 +5819,7 @@
         <v>0</v>
       </c>
       <c r="AQ18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1510.9985160214314</v>
       </c>
       <c r="AS18">
@@ -4925,15 +5875,15 @@
         <v>3.0039090000000001E-2</v>
       </c>
       <c r="BL18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1375.9736485714286</v>
       </c>
       <c r="BN18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO18" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP18" s="3">
@@ -4955,7 +5905,7 @@
         <v>5.7098599999999998E-3</v>
       </c>
       <c r="BV18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1339.6866297841727</v>
       </c>
       <c r="BX18">
@@ -4980,11 +5930,61 @@
         <v>0.75318819415173699</v>
       </c>
       <c r="CE18">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1336.5184635327957</v>
       </c>
+      <c r="CG18">
+        <v>15</v>
+      </c>
+      <c r="CH18">
+        <v>1331.32397729493</v>
+      </c>
+      <c r="CI18">
+        <v>3.8192921771887899E-2</v>
+      </c>
+      <c r="CJ18">
+        <v>0.25305423498319601</v>
+      </c>
+      <c r="CK18">
+        <v>1</v>
+      </c>
+      <c r="CL18">
+        <v>6.6739298723252696E-3</v>
+      </c>
+      <c r="CM18">
+        <v>0.36908079349563899</v>
+      </c>
+      <c r="CN18">
+        <v>0</v>
+      </c>
+      <c r="CO18">
+        <f t="shared" si="18"/>
+        <v>1343.9371159810614</v>
+      </c>
+      <c r="CQ18">
+        <v>15</v>
+      </c>
+      <c r="CR18">
+        <v>1366.48074486007</v>
+      </c>
+      <c r="CS18">
+        <v>0.70170891672241298</v>
+      </c>
+      <c r="CT18">
+        <v>0.196038194811645</v>
+      </c>
+      <c r="CU18">
+        <v>1</v>
+      </c>
+      <c r="CV18">
+        <v>2.05768241154674E-2</v>
+      </c>
+      <c r="CW18">
+        <f t="shared" si="19"/>
+        <v>1374.7685146442427</v>
+      </c>
     </row>
-    <row r="19" spans="1:83">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
@@ -5067,7 +6067,7 @@
       </c>
       <c r="AC19">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD19">
         <f t="shared" si="7"/>
@@ -5081,6 +6081,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG19">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AH19">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI19">
         <v>16</v>
       </c>
@@ -5106,7 +6114,7 @@
         <v>5.0058361152044503E-5</v>
       </c>
       <c r="AQ19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>555.91806425423135</v>
       </c>
       <c r="AS19">
@@ -5162,15 +6170,15 @@
         <v>3.730116E-2</v>
       </c>
       <c r="BL19">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>455.1773415714286</v>
       </c>
       <c r="BN19">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO19" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP19" s="3">
@@ -5192,7 +6200,7 @@
         <v>2.49614E-3</v>
       </c>
       <c r="BV19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>461.01691678417268</v>
       </c>
       <c r="BX19">
@@ -5217,11 +6225,61 @@
         <v>0.96163846878299897</v>
       </c>
       <c r="CE19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>453.65868362818463</v>
       </c>
+      <c r="CG19">
+        <v>16</v>
+      </c>
+      <c r="CH19">
+        <v>438.43470471005497</v>
+      </c>
+      <c r="CI19">
+        <v>1.8466122887919802E-2</v>
+      </c>
+      <c r="CJ19">
+        <v>0.41299104747947402</v>
+      </c>
+      <c r="CK19">
+        <v>1</v>
+      </c>
+      <c r="CL19">
+        <v>3.4039133178603901E-3</v>
+      </c>
+      <c r="CM19">
+        <v>0.356597147034732</v>
+      </c>
+      <c r="CN19">
+        <v>0</v>
+      </c>
+      <c r="CO19">
+        <f t="shared" si="18"/>
+        <v>451.04784339618635</v>
+      </c>
+      <c r="CQ19">
+        <v>16</v>
+      </c>
+      <c r="CR19">
+        <v>701.90978544848497</v>
+      </c>
+      <c r="CS19">
+        <v>9.5970671942496602E-2</v>
+      </c>
+      <c r="CT19">
+        <v>0.20052157234149301</v>
+      </c>
+      <c r="CU19">
+        <v>1</v>
+      </c>
+      <c r="CV19">
+        <v>0</v>
+      </c>
+      <c r="CW19">
+        <f t="shared" si="19"/>
+        <v>710.19755523265758</v>
+      </c>
     </row>
-    <row r="20" spans="1:83">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
@@ -5318,6 +6376,14 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
+      <c r="AG20">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH20">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI20">
         <v>17</v>
       </c>
@@ -5343,7 +6409,7 @@
         <v>3.16617851033649E-3</v>
       </c>
       <c r="AQ20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1125.9929745979514</v>
       </c>
       <c r="AS20">
@@ -5399,15 +6465,15 @@
         <v>6.4879200000000003E-3</v>
       </c>
       <c r="BL20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1061.9400985714285</v>
       </c>
       <c r="BN20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO20" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP20" s="3">
@@ -5429,7 +6495,7 @@
         <v>9.1253500000000008E-3</v>
       </c>
       <c r="BV20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1015.2907697841727</v>
       </c>
       <c r="BX20">
@@ -5454,11 +6520,61 @@
         <v>0.89266804644332398</v>
       </c>
       <c r="CE20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1010.7740349694457</v>
       </c>
+      <c r="CG20">
+        <v>17</v>
+      </c>
+      <c r="CH20">
+        <v>1008.15989311806</v>
+      </c>
+      <c r="CI20">
+        <v>2.0265967685290001E-2</v>
+      </c>
+      <c r="CJ20">
+        <v>0.25159358755327599</v>
+      </c>
+      <c r="CK20">
+        <v>1</v>
+      </c>
+      <c r="CL20">
+        <v>8.6966823885079904E-3</v>
+      </c>
+      <c r="CM20">
+        <v>1</v>
+      </c>
+      <c r="CN20">
+        <v>0</v>
+      </c>
+      <c r="CO20">
+        <f t="shared" si="18"/>
+        <v>1020.7730318041914</v>
+      </c>
+      <c r="CQ20">
+        <v>17</v>
+      </c>
+      <c r="CR20">
+        <v>1063.51439953621</v>
+      </c>
+      <c r="CS20">
+        <v>0.26768611964442401</v>
+      </c>
+      <c r="CT20">
+        <v>0.23474990872546</v>
+      </c>
+      <c r="CU20">
+        <v>1</v>
+      </c>
+      <c r="CV20">
+        <v>1.23898869013731E-2</v>
+      </c>
+      <c r="CW20">
+        <f t="shared" si="19"/>
+        <v>1071.8021693203827</v>
+      </c>
     </row>
-    <row r="21" spans="1:83">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
@@ -5555,6 +6671,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG21">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH21">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI21">
         <v>18</v>
       </c>
@@ -5580,7 +6704,7 @@
         <v>6.7046788472800998E-3</v>
       </c>
       <c r="AQ21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1920.0215078977515</v>
       </c>
       <c r="AS21">
@@ -5636,15 +6760,15 @@
         <v>2.6256450000000001E-2</v>
       </c>
       <c r="BL21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1914.1050885714285</v>
       </c>
       <c r="BN21">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO21" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP21" s="3">
@@ -5666,7 +6790,7 @@
         <v>1.170291E-2</v>
       </c>
       <c r="BV21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1910.7142197841727</v>
       </c>
       <c r="BX21">
@@ -5691,11 +6815,61 @@
         <v>0.117794113486674</v>
       </c>
       <c r="CE21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1906.2760803088258</v>
       </c>
+      <c r="CG21">
+        <v>18</v>
+      </c>
+      <c r="CH21">
+        <v>1882.16499760478</v>
+      </c>
+      <c r="CI21">
+        <v>2.0932613816704401E-2</v>
+      </c>
+      <c r="CJ21">
+        <v>0.10693473226174</v>
+      </c>
+      <c r="CK21">
+        <v>1</v>
+      </c>
+      <c r="CL21">
+        <v>3.0573594975778101E-4</v>
+      </c>
+      <c r="CM21">
+        <v>1</v>
+      </c>
+      <c r="CN21">
+        <v>7.1414480001892101E-4</v>
+      </c>
+      <c r="CO21">
+        <f t="shared" si="18"/>
+        <v>1894.7781362909113</v>
+      </c>
+      <c r="CQ21">
+        <v>18</v>
+      </c>
+      <c r="CR21">
+        <v>1892.04872256678</v>
+      </c>
+      <c r="CS21">
+        <v>0.11867931788619999</v>
+      </c>
+      <c r="CT21">
+        <v>0.209884094858801</v>
+      </c>
+      <c r="CU21">
+        <v>1</v>
+      </c>
+      <c r="CV21">
+        <v>0</v>
+      </c>
+      <c r="CW21">
+        <f t="shared" si="19"/>
+        <v>1900.3364923509528</v>
+      </c>
     </row>
-    <row r="22" spans="1:83">
+    <row r="22" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
@@ -5792,6 +6966,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH22">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI22">
         <v>19</v>
       </c>
@@ -5817,7 +6999,7 @@
         <v>3.9914528542376003E-3</v>
       </c>
       <c r="AQ22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>695.73417801323035</v>
       </c>
       <c r="AS22">
@@ -5873,15 +7055,15 @@
         <v>1.313137E-2</v>
       </c>
       <c r="BL22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>535.95648757142862</v>
       </c>
       <c r="BN22">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO22" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP22" s="3">
@@ -5903,7 +7085,7 @@
         <v>8.38765E-3</v>
       </c>
       <c r="BV22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>515.21917778417264</v>
       </c>
       <c r="BX22">
@@ -5928,11 +7110,61 @@
         <v>0.83341407219184105</v>
       </c>
       <c r="CE22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>506.95770343110564</v>
       </c>
+      <c r="CG22">
+        <v>19</v>
+      </c>
+      <c r="CH22">
+        <v>497.47147806294203</v>
+      </c>
+      <c r="CI22">
+        <v>3.0633438504594299E-2</v>
+      </c>
+      <c r="CJ22">
+        <v>0.298661091911604</v>
+      </c>
+      <c r="CK22">
+        <v>1</v>
+      </c>
+      <c r="CL22">
+        <v>8.8990782351395705E-3</v>
+      </c>
+      <c r="CM22">
+        <v>0.85096622266147304</v>
+      </c>
+      <c r="CN22">
+        <v>2.1019294833146698E-2</v>
+      </c>
+      <c r="CO22">
+        <f t="shared" si="18"/>
+        <v>510.0846167490734</v>
+      </c>
+      <c r="CQ22">
+        <v>19</v>
+      </c>
+      <c r="CR22">
+        <v>551.053931683207</v>
+      </c>
+      <c r="CS22">
+        <v>0.467862950061327</v>
+      </c>
+      <c r="CT22">
+        <v>0.28627362685562602</v>
+      </c>
+      <c r="CU22">
+        <v>1</v>
+      </c>
+      <c r="CV22">
+        <v>1.7437585502825301E-2</v>
+      </c>
+      <c r="CW22">
+        <f t="shared" si="19"/>
+        <v>559.34170146737961</v>
+      </c>
     </row>
-    <row r="23" spans="1:83" s="2" customFormat="1">
+    <row r="23" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
@@ -6030,6 +7262,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG23">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH23">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI23">
         <v>20</v>
       </c>
@@ -6055,7 +7295,7 @@
         <v>0</v>
       </c>
       <c r="AQ23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1200.4842793119615</v>
       </c>
       <c r="AS23">
@@ -6111,15 +7351,15 @@
         <v>1.071101E-2</v>
       </c>
       <c r="BL23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1122.5551485714286</v>
       </c>
       <c r="BN23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BO23" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP23" s="3">
@@ -6141,7 +7381,7 @@
         <v>0</v>
       </c>
       <c r="BV23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1139.7824397841728</v>
       </c>
       <c r="BX23">
@@ -6166,11 +7406,61 @@
         <v>0.13073143793935099</v>
       </c>
       <c r="CE23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1126.5086784933658</v>
       </c>
+      <c r="CG23">
+        <v>20</v>
+      </c>
+      <c r="CH23">
+        <v>1107.3393843762799</v>
+      </c>
+      <c r="CI23">
+        <v>1.6553006870076999E-2</v>
+      </c>
+      <c r="CJ23">
+        <v>0.271640826376078</v>
+      </c>
+      <c r="CK23">
+        <v>1</v>
+      </c>
+      <c r="CL23">
+        <v>0</v>
+      </c>
+      <c r="CM23">
+        <v>9.7700540025135493E-2</v>
+      </c>
+      <c r="CN23">
+        <v>0</v>
+      </c>
+      <c r="CO23">
+        <f t="shared" si="18"/>
+        <v>1119.9525230624113</v>
+      </c>
+      <c r="CQ23">
+        <v>20</v>
+      </c>
+      <c r="CR23">
+        <v>1234.5186831542801</v>
+      </c>
+      <c r="CS23">
+        <v>7.8915364876438299E-2</v>
+      </c>
+      <c r="CT23">
+        <v>0.19985990332959799</v>
+      </c>
+      <c r="CU23">
+        <v>1</v>
+      </c>
+      <c r="CV23">
+        <v>0</v>
+      </c>
+      <c r="CW23">
+        <f t="shared" si="19"/>
+        <v>1242.8064529384528</v>
+      </c>
     </row>
-    <row r="24" spans="1:83">
+    <row r="24" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
@@ -6267,6 +7557,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG24">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH24">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI24">
         <v>21</v>
       </c>
@@ -6292,7 +7590,7 @@
         <v>3.6932834847521502E-3</v>
       </c>
       <c r="AQ24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1164.7032112442914</v>
       </c>
       <c r="AS24">
@@ -6348,15 +7646,15 @@
         <v>3.0027600000000002E-2</v>
       </c>
       <c r="BL24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1104.9961785714286</v>
       </c>
       <c r="BN24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO24" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP24" s="3">
@@ -6378,7 +7676,7 @@
         <v>4.0800899999999998E-3</v>
       </c>
       <c r="BV24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1094.4659397841726</v>
       </c>
       <c r="BX24">
@@ -6403,11 +7701,61 @@
         <v>0.94633145110703298</v>
       </c>
       <c r="CE24">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1079.5451989367757</v>
       </c>
+      <c r="CG24">
+        <v>21</v>
+      </c>
+      <c r="CH24">
+        <v>1066.93244473963</v>
+      </c>
+      <c r="CI24">
+        <v>3.5890293364817902E-2</v>
+      </c>
+      <c r="CJ24">
+        <v>0.22923193329069799</v>
+      </c>
+      <c r="CK24">
+        <v>1</v>
+      </c>
+      <c r="CL24">
+        <v>7.8882163928771492E-3</v>
+      </c>
+      <c r="CM24">
+        <v>0.17784209899878001</v>
+      </c>
+      <c r="CN24">
+        <v>0</v>
+      </c>
+      <c r="CO24">
+        <f t="shared" si="18"/>
+        <v>1079.5455834257614</v>
+      </c>
+      <c r="CQ24">
+        <v>21</v>
+      </c>
+      <c r="CR24">
+        <v>1087.6329041567301</v>
+      </c>
+      <c r="CS24">
+        <v>0.40490397633789699</v>
+      </c>
+      <c r="CT24">
+        <v>0.214430982515703</v>
+      </c>
+      <c r="CU24">
+        <v>1</v>
+      </c>
+      <c r="CV24">
+        <v>1.0123029860469399E-2</v>
+      </c>
+      <c r="CW24">
+        <f t="shared" si="19"/>
+        <v>1095.9206739409028</v>
+      </c>
     </row>
-    <row r="25" spans="1:83">
+    <row r="25" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>22</v>
       </c>
@@ -6504,6 +7852,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH25">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI25">
         <v>22</v>
       </c>
@@ -6529,7 +7885,7 @@
         <v>7.0641183302977103E-4</v>
       </c>
       <c r="AQ25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>967.6150311743944</v>
       </c>
       <c r="AS25">
@@ -6585,15 +7941,15 @@
         <v>1.3830500000000001E-2</v>
       </c>
       <c r="BL25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>912.94836657142855</v>
       </c>
       <c r="BN25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO25" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP25" s="3">
@@ -6615,7 +7971,7 @@
         <v>5.2050600000000001E-3</v>
       </c>
       <c r="BV25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>913.52001278417265</v>
       </c>
       <c r="BX25">
@@ -6640,11 +7996,61 @@
         <v>6.4978579102946493E-2</v>
       </c>
       <c r="CE25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>910.21176849556161</v>
       </c>
+      <c r="CG25">
+        <v>22</v>
+      </c>
+      <c r="CH25">
+        <v>898.18630950090096</v>
+      </c>
+      <c r="CI25">
+        <v>2.3838747170836502E-2</v>
+      </c>
+      <c r="CJ25">
+        <v>0.24306922043211199</v>
+      </c>
+      <c r="CK25">
+        <v>1</v>
+      </c>
+      <c r="CL25">
+        <v>4.2863317482380097E-3</v>
+      </c>
+      <c r="CM25">
+        <v>0.204608611766946</v>
+      </c>
+      <c r="CN25">
+        <v>0</v>
+      </c>
+      <c r="CO25">
+        <f t="shared" si="18"/>
+        <v>910.79944818703234</v>
+      </c>
+      <c r="CQ25">
+        <v>22</v>
+      </c>
+      <c r="CR25">
+        <v>1020.0816508764</v>
+      </c>
+      <c r="CS25">
+        <v>0.30753826521321598</v>
+      </c>
+      <c r="CT25">
+        <v>0.14757772309555101</v>
+      </c>
+      <c r="CU25">
+        <v>1</v>
+      </c>
+      <c r="CV25">
+        <v>9.6331428846047201E-3</v>
+      </c>
+      <c r="CW25">
+        <f t="shared" si="19"/>
+        <v>1028.3694206605726</v>
+      </c>
     </row>
-    <row r="26" spans="1:83">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>23</v>
       </c>
@@ -6741,6 +8147,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI26">
         <v>23</v>
       </c>
@@ -6766,7 +8180,7 @@
         <v>0</v>
       </c>
       <c r="AQ26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1118.8847164971114</v>
       </c>
       <c r="AS26">
@@ -6822,15 +8236,15 @@
         <v>3.0272799999999999E-2</v>
       </c>
       <c r="BL26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1062.6371785714286</v>
       </c>
       <c r="BN26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO26" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP26" s="3">
@@ -6852,7 +8266,7 @@
         <v>3.2112999999999998E-3</v>
       </c>
       <c r="BV26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1053.7629597841728</v>
       </c>
       <c r="BX26">
@@ -6877,11 +8291,61 @@
         <v>0.98739919626232198</v>
       </c>
       <c r="CE26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1051.5931349378257</v>
       </c>
+      <c r="CG26">
+        <v>23</v>
+      </c>
+      <c r="CH26">
+        <v>1043.8797422115199</v>
+      </c>
+      <c r="CI26">
+        <v>2.1054859228923799E-2</v>
+      </c>
+      <c r="CJ26">
+        <v>0.221530278625787</v>
+      </c>
+      <c r="CK26">
+        <v>1</v>
+      </c>
+      <c r="CL26">
+        <v>4.77130889976227E-3</v>
+      </c>
+      <c r="CM26">
+        <v>0.54758099829756601</v>
+      </c>
+      <c r="CN26">
+        <v>0</v>
+      </c>
+      <c r="CO26">
+        <f t="shared" si="18"/>
+        <v>1056.4928808976513</v>
+      </c>
+      <c r="CQ26">
+        <v>23</v>
+      </c>
+      <c r="CR26">
+        <v>1070.6263941641801</v>
+      </c>
+      <c r="CS26">
+        <v>0.42498923913678299</v>
+      </c>
+      <c r="CT26">
+        <v>0.20749174202471901</v>
+      </c>
+      <c r="CU26">
+        <v>1</v>
+      </c>
+      <c r="CV26">
+        <v>1.8683827786759599E-2</v>
+      </c>
+      <c r="CW26">
+        <f t="shared" si="19"/>
+        <v>1078.9141639483528</v>
+      </c>
     </row>
-    <row r="27" spans="1:83">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>24</v>
       </c>
@@ -6956,7 +8420,7 @@
       </c>
       <c r="AA27">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB27">
         <f t="shared" si="5"/>
@@ -6978,6 +8442,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG27">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AH27">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI27">
         <v>24</v>
       </c>
@@ -7003,7 +8475,7 @@
         <v>4.9339599272811797E-3</v>
       </c>
       <c r="AQ27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>999.37264829190042</v>
       </c>
       <c r="AS27">
@@ -7059,15 +8531,15 @@
         <v>1.379678E-2</v>
       </c>
       <c r="BL27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>956.07284857142861</v>
       </c>
       <c r="BN27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BO27" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP27" s="3">
@@ -7089,7 +8561,7 @@
         <v>3.7196899999999999E-3</v>
       </c>
       <c r="BV27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>963.73892978417257</v>
       </c>
       <c r="BX27">
@@ -7114,11 +8586,61 @@
         <v>0.78583358968345896</v>
       </c>
       <c r="CE27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>959.0000137049426</v>
       </c>
+      <c r="CG27">
+        <v>24</v>
+      </c>
+      <c r="CH27">
+        <v>940.66804231306401</v>
+      </c>
+      <c r="CI27">
+        <v>2.4351236192978899E-2</v>
+      </c>
+      <c r="CJ27">
+        <v>0.17176826643007301</v>
+      </c>
+      <c r="CK27">
+        <v>0.98899090941012402</v>
+      </c>
+      <c r="CL27">
+        <v>2.2530917268209498E-3</v>
+      </c>
+      <c r="CM27">
+        <v>0.77896862216699603</v>
+      </c>
+      <c r="CN27">
+        <v>3.5932512104094899E-2</v>
+      </c>
+      <c r="CO27">
+        <f t="shared" si="18"/>
+        <v>953.28118099919539</v>
+      </c>
+      <c r="CQ27">
+        <v>24</v>
+      </c>
+      <c r="CR27">
+        <v>1004.82672177385</v>
+      </c>
+      <c r="CS27">
+        <v>0.184143768477987</v>
+      </c>
+      <c r="CT27">
+        <v>0.210008432283802</v>
+      </c>
+      <c r="CU27">
+        <v>1</v>
+      </c>
+      <c r="CV27">
+        <v>2.4259741848499999E-3</v>
+      </c>
+      <c r="CW27">
+        <f t="shared" si="19"/>
+        <v>1013.1144915580226</v>
+      </c>
     </row>
-    <row r="28" spans="1:83">
+    <row r="28" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>25</v>
       </c>
@@ -7215,6 +8737,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH28">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI28">
         <v>25</v>
       </c>
@@ -7240,7 +8770,7 @@
         <v>4.2349650311626899E-3</v>
       </c>
       <c r="AQ28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>865.13078426492837</v>
       </c>
       <c r="AS28">
@@ -7296,15 +8826,15 @@
         <v>3.1708229999999997E-2</v>
       </c>
       <c r="BL28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>812.25329257142857</v>
       </c>
       <c r="BN28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO28" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP28" s="3">
@@ -7326,7 +8856,7 @@
         <v>1.189431E-2</v>
       </c>
       <c r="BV28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>769.53660778417259</v>
       </c>
       <c r="BX28">
@@ -7351,11 +8881,61 @@
         <v>0.94771440338885904</v>
       </c>
       <c r="CE28">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>763.19402400405568</v>
       </c>
+      <c r="CG28">
+        <v>25</v>
+      </c>
+      <c r="CH28">
+        <v>749.38957869154297</v>
+      </c>
+      <c r="CI28">
+        <v>2.0107496773898399E-2</v>
+      </c>
+      <c r="CJ28">
+        <v>0.43381782324523099</v>
+      </c>
+      <c r="CK28">
+        <v>1</v>
+      </c>
+      <c r="CL28">
+        <v>1.48138842518087E-2</v>
+      </c>
+      <c r="CM28">
+        <v>0.397999644476771</v>
+      </c>
+      <c r="CN28">
+        <v>3.1856140124859201E-3</v>
+      </c>
+      <c r="CO28">
+        <f t="shared" si="18"/>
+        <v>762.00271737767434</v>
+      </c>
+      <c r="CQ28">
+        <v>25</v>
+      </c>
+      <c r="CR28">
+        <v>807.82085999253002</v>
+      </c>
+      <c r="CS28">
+        <v>0.36499676724913699</v>
+      </c>
+      <c r="CT28">
+        <v>0.32850342240160102</v>
+      </c>
+      <c r="CU28">
+        <v>1</v>
+      </c>
+      <c r="CV28">
+        <v>3.1426489150716802E-2</v>
+      </c>
+      <c r="CW28">
+        <f t="shared" si="19"/>
+        <v>816.10862977670263</v>
+      </c>
     </row>
-    <row r="29" spans="1:83" s="2" customFormat="1">
+    <row r="29" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>26</v>
       </c>
@@ -7447,12 +9027,20 @@
       </c>
       <c r="AE29">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG29">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AH29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI29">
         <v>26</v>
       </c>
@@ -7478,7 +9066,7 @@
         <v>0</v>
       </c>
       <c r="AQ29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1933.1757465742915</v>
       </c>
       <c r="AS29">
@@ -7534,15 +9122,15 @@
         <v>2.549887E-2</v>
       </c>
       <c r="BL29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1857.6301185714285</v>
       </c>
       <c r="BN29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO29" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP29" s="3">
@@ -7564,7 +9152,7 @@
         <v>2.5349960000000001E-2</v>
       </c>
       <c r="BV29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1903.9252197841727</v>
       </c>
       <c r="BX29">
@@ -7589,11 +9177,61 @@
         <v>0.343152198435419</v>
       </c>
       <c r="CE29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1838.6981815187457</v>
       </c>
+      <c r="CG29">
+        <v>26</v>
+      </c>
+      <c r="CH29">
+        <v>1807.0673928505</v>
+      </c>
+      <c r="CI29">
+        <v>4.05799857926184E-2</v>
+      </c>
+      <c r="CJ29">
+        <v>0.164023441985234</v>
+      </c>
+      <c r="CK29">
+        <v>1</v>
+      </c>
+      <c r="CL29">
+        <v>2.2911498497076199E-3</v>
+      </c>
+      <c r="CM29">
+        <v>1</v>
+      </c>
+      <c r="CN29">
+        <v>0</v>
+      </c>
+      <c r="CO29">
+        <f t="shared" si="18"/>
+        <v>1819.6805315366314</v>
+      </c>
+      <c r="CQ29">
+        <v>26</v>
+      </c>
+      <c r="CR29">
+        <v>1867.3988714649599</v>
+      </c>
+      <c r="CS29">
+        <v>0.66467795711078603</v>
+      </c>
+      <c r="CT29">
+        <v>0.12899238937890201</v>
+      </c>
+      <c r="CU29">
+        <v>1</v>
+      </c>
+      <c r="CV29">
+        <v>6.8983314935404296E-3</v>
+      </c>
+      <c r="CW29">
+        <f t="shared" si="19"/>
+        <v>1875.6866412491327</v>
+      </c>
     </row>
-    <row r="30" spans="1:83">
+    <row r="30" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>27</v>
       </c>
@@ -7690,6 +9328,14 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
+      <c r="AG30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH30">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI30">
         <v>27</v>
       </c>
@@ -7715,7 +9361,7 @@
         <v>0</v>
       </c>
       <c r="AQ30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>943.69932783804836</v>
       </c>
       <c r="AS30">
@@ -7771,15 +9417,15 @@
         <v>2.591978E-2</v>
       </c>
       <c r="BL30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>753.57543557142856</v>
       </c>
       <c r="BN30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO30" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP30" s="3">
@@ -7801,7 +9447,7 @@
         <v>7.39217E-3</v>
       </c>
       <c r="BV30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>732.19212078417263</v>
       </c>
       <c r="BX30">
@@ -7826,11 +9472,61 @@
         <v>0.91728842055096904</v>
       </c>
       <c r="CE30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>694.04252586220559</v>
       </c>
+      <c r="CG30">
+        <v>27</v>
+      </c>
+      <c r="CH30">
+        <v>691.84513330689003</v>
+      </c>
+      <c r="CI30">
+        <v>2.3877900888571699E-2</v>
+      </c>
+      <c r="CJ30">
+        <v>0.34190364009580299</v>
+      </c>
+      <c r="CK30">
+        <v>1</v>
+      </c>
+      <c r="CL30">
+        <v>7.0612487290772604E-3</v>
+      </c>
+      <c r="CM30">
+        <v>1</v>
+      </c>
+      <c r="CN30">
+        <v>2.7526893459379299E-2</v>
+      </c>
+      <c r="CO30">
+        <f t="shared" si="18"/>
+        <v>704.45827199302141</v>
+      </c>
+      <c r="CQ30">
+        <v>27</v>
+      </c>
+      <c r="CR30">
+        <v>772.23025732765802</v>
+      </c>
+      <c r="CS30">
+        <v>0.48589041911560099</v>
+      </c>
+      <c r="CT30">
+        <v>0.28620253143569202</v>
+      </c>
+      <c r="CU30">
+        <v>1</v>
+      </c>
+      <c r="CV30">
+        <v>1.00459089611773E-2</v>
+      </c>
+      <c r="CW30">
+        <f t="shared" si="19"/>
+        <v>780.51802711183063</v>
+      </c>
     </row>
-    <row r="31" spans="1:83">
+    <row r="31" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>28</v>
       </c>
@@ -7927,6 +9623,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH31">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI31">
         <v>28</v>
       </c>
@@ -7952,7 +9656,7 @@
         <v>0</v>
       </c>
       <c r="AQ31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>951.54230862544932</v>
       </c>
       <c r="AS31">
@@ -8008,15 +9712,15 @@
         <v>4.9921000000000004E-4</v>
       </c>
       <c r="BL31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>804.70652057142854</v>
       </c>
       <c r="BN31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO31" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BP31" s="3">
@@ -8038,7 +9742,7 @@
         <v>2.3951100000000002E-3</v>
       </c>
       <c r="BV31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>785.85849578417265</v>
       </c>
       <c r="BX31">
@@ -8063,11 +9767,61 @@
         <v>0.80956842191327305</v>
       </c>
       <c r="CE31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>792.6678611053286</v>
       </c>
+      <c r="CG31">
+        <v>28</v>
+      </c>
+      <c r="CH31">
+        <v>783.03202907164496</v>
+      </c>
+      <c r="CI31">
+        <v>2.2067548673766198E-2</v>
+      </c>
+      <c r="CJ31">
+        <v>0.31834865634217602</v>
+      </c>
+      <c r="CK31">
+        <v>1</v>
+      </c>
+      <c r="CL31">
+        <v>3.72722668695894E-3</v>
+      </c>
+      <c r="CM31">
+        <v>0.46798819527413998</v>
+      </c>
+      <c r="CN31">
+        <v>0</v>
+      </c>
+      <c r="CO31">
+        <f t="shared" si="18"/>
+        <v>795.64516775777633</v>
+      </c>
+      <c r="CQ31">
+        <v>28</v>
+      </c>
+      <c r="CR31">
+        <v>960.471388438963</v>
+      </c>
+      <c r="CS31">
+        <v>0.35955734551942498</v>
+      </c>
+      <c r="CT31">
+        <v>0.21266113759382199</v>
+      </c>
+      <c r="CU31">
+        <v>1</v>
+      </c>
+      <c r="CV31">
+        <v>6.00406375206557E-3</v>
+      </c>
+      <c r="CW31">
+        <f t="shared" si="19"/>
+        <v>968.75915822313561</v>
+      </c>
     </row>
-    <row r="32" spans="1:83">
+    <row r="32" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>29</v>
       </c>
@@ -8164,6 +9918,14 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
+      <c r="AG32">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH32">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI32">
         <v>29</v>
       </c>
@@ -8189,7 +9951,7 @@
         <v>2.2522505941462601E-4</v>
       </c>
       <c r="AQ32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1555.4717452455013</v>
       </c>
       <c r="AS32">
@@ -8245,15 +10007,15 @@
         <v>4.4399260000000003E-2</v>
       </c>
       <c r="BL32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1298.5770485714286</v>
       </c>
       <c r="BN32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO32" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP32" s="3">
@@ -8275,7 +10037,7 @@
         <v>1.1183220000000001E-2</v>
       </c>
       <c r="BV32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1299.2451997841727</v>
       </c>
       <c r="BX32">
@@ -8300,11 +10062,61 @@
         <v>0.63133086124156801</v>
       </c>
       <c r="CE32">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1240.7569727206658</v>
       </c>
+      <c r="CG32">
+        <v>29</v>
+      </c>
+      <c r="CH32">
+        <v>1258.1184197478999</v>
+      </c>
+      <c r="CI32">
+        <v>0.26526501132694602</v>
+      </c>
+      <c r="CJ32">
+        <v>0.25037820557614199</v>
+      </c>
+      <c r="CK32">
+        <v>1</v>
+      </c>
+      <c r="CL32">
+        <v>1.7377154913007099E-2</v>
+      </c>
+      <c r="CM32">
+        <v>0.20837100700549999</v>
+      </c>
+      <c r="CN32">
+        <v>0</v>
+      </c>
+      <c r="CO32">
+        <f t="shared" si="18"/>
+        <v>1270.7315584340313</v>
+      </c>
+      <c r="CQ32">
+        <v>29</v>
+      </c>
+      <c r="CR32">
+        <v>1280.77848719077</v>
+      </c>
+      <c r="CS32">
+        <v>0.75639538986928401</v>
+      </c>
+      <c r="CT32">
+        <v>0.277951196965946</v>
+      </c>
+      <c r="CU32">
+        <v>1</v>
+      </c>
+      <c r="CV32">
+        <v>1.46171500345369E-2</v>
+      </c>
+      <c r="CW32">
+        <f t="shared" si="19"/>
+        <v>1289.0662569749427</v>
+      </c>
     </row>
-    <row r="33" spans="1:83">
+    <row r="33" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>30</v>
       </c>
@@ -8401,6 +10213,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG33">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH33">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI33">
         <v>30</v>
       </c>
@@ -8426,7 +10246,7 @@
         <v>0</v>
       </c>
       <c r="AQ33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1492.8125076619515</v>
       </c>
       <c r="AS33">
@@ -8482,15 +10302,15 @@
         <v>2.3769269999999999E-2</v>
       </c>
       <c r="BL33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1389.0064885714287</v>
       </c>
       <c r="BN33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO33" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP33" s="3">
@@ -8512,7 +10332,7 @@
         <v>0</v>
       </c>
       <c r="BV33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1420.6464197841726</v>
       </c>
       <c r="BX33">
@@ -8537,11 +10357,61 @@
         <v>3.10134154003887E-2</v>
       </c>
       <c r="CE33">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1374.7220396423857</v>
       </c>
+      <c r="CG33">
+        <v>30</v>
+      </c>
+      <c r="CH33">
+        <v>1341.89892354619</v>
+      </c>
+      <c r="CI33">
+        <v>8.1816809503815299E-2</v>
+      </c>
+      <c r="CJ33">
+        <v>0.260690062958227</v>
+      </c>
+      <c r="CK33">
+        <v>1</v>
+      </c>
+      <c r="CL33">
+        <v>3.14958916180957E-3</v>
+      </c>
+      <c r="CM33">
+        <v>4.2145041224265899E-2</v>
+      </c>
+      <c r="CN33">
+        <v>0</v>
+      </c>
+      <c r="CO33">
+        <f t="shared" si="18"/>
+        <v>1354.5120622323213</v>
+      </c>
+      <c r="CQ33">
+        <v>30</v>
+      </c>
+      <c r="CR33">
+        <v>1356.8487821414601</v>
+      </c>
+      <c r="CS33">
+        <v>4.2476197125436897E-2</v>
+      </c>
+      <c r="CT33">
+        <v>0.48889236610478098</v>
+      </c>
+      <c r="CU33">
+        <v>1</v>
+      </c>
+      <c r="CV33">
+        <v>0</v>
+      </c>
+      <c r="CW33">
+        <f t="shared" si="19"/>
+        <v>1365.1365519256328</v>
+      </c>
     </row>
-    <row r="34" spans="1:83">
+    <row r="34" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>31</v>
       </c>
@@ -8638,6 +10508,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH34">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI34">
         <v>31</v>
       </c>
@@ -8663,7 +10541,7 @@
         <v>3.1807481714730902E-4</v>
       </c>
       <c r="AQ34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1146.7525835518513</v>
       </c>
       <c r="AS34">
@@ -8719,15 +10597,15 @@
         <v>8.8369699999999995E-3</v>
       </c>
       <c r="BL34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>949.48137257142855</v>
       </c>
       <c r="BN34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO34" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP34" s="3">
@@ -8749,7 +10627,7 @@
         <v>1.00979E-2</v>
       </c>
       <c r="BV34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>952.65348978417262</v>
       </c>
       <c r="BX34">
@@ -8774,11 +10652,61 @@
         <v>0.95703079016194803</v>
       </c>
       <c r="CE34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>914.41754492588666</v>
       </c>
+      <c r="CG34">
+        <v>31</v>
+      </c>
+      <c r="CH34">
+        <v>898.74545101036199</v>
+      </c>
+      <c r="CI34">
+        <v>4.5553068810292599E-2</v>
+      </c>
+      <c r="CJ34">
+        <v>0.23596711247534</v>
+      </c>
+      <c r="CK34">
+        <v>1</v>
+      </c>
+      <c r="CL34">
+        <v>5.6595216256657196E-3</v>
+      </c>
+      <c r="CM34">
+        <v>0.88230945686100903</v>
+      </c>
+      <c r="CN34">
+        <v>0.05</v>
+      </c>
+      <c r="CO34">
+        <f t="shared" si="18"/>
+        <v>911.35858969649337</v>
+      </c>
+      <c r="CQ34">
+        <v>31</v>
+      </c>
+      <c r="CR34">
+        <v>964.89521399353805</v>
+      </c>
+      <c r="CS34">
+        <v>0.63441054512529005</v>
+      </c>
+      <c r="CT34">
+        <v>0.24407556143304601</v>
+      </c>
+      <c r="CU34">
+        <v>1</v>
+      </c>
+      <c r="CV34">
+        <v>1.6336955641049401E-2</v>
+      </c>
+      <c r="CW34">
+        <f t="shared" si="19"/>
+        <v>973.18298377771066</v>
+      </c>
     </row>
-    <row r="35" spans="1:83">
+    <row r="35" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>32</v>
       </c>
@@ -8875,6 +10803,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG35">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH35">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI35">
         <v>32</v>
       </c>
@@ -8900,7 +10836,7 @@
         <v>0</v>
       </c>
       <c r="AQ35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1618.4010583787615</v>
       </c>
       <c r="AS35">
@@ -8956,15 +10892,15 @@
         <v>1.529553E-2</v>
       </c>
       <c r="BL35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1594.2908085714287</v>
       </c>
       <c r="BN35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BO35" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BP35" s="3">
@@ -8986,7 +10922,7 @@
         <v>0</v>
       </c>
       <c r="BV35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1596.4022197841728</v>
       </c>
       <c r="BX35">
@@ -9011,11 +10947,61 @@
         <v>0.72269794614477501</v>
       </c>
       <c r="CE35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1598.2931573804858</v>
       </c>
+      <c r="CG35">
+        <v>32</v>
+      </c>
+      <c r="CH35">
+        <v>1584.0278698223599</v>
+      </c>
+      <c r="CI35">
+        <v>0.99942042269162101</v>
+      </c>
+      <c r="CJ35">
+        <v>1.44922526426266</v>
+      </c>
+      <c r="CK35">
+        <v>0.99943630169832898</v>
+      </c>
+      <c r="CL35">
+        <v>4.10816422880013E-3</v>
+      </c>
+      <c r="CM35" s="1">
+        <v>5.8879053967172897E-5</v>
+      </c>
+      <c r="CN35">
+        <v>0</v>
+      </c>
+      <c r="CO35">
+        <f t="shared" si="18"/>
+        <v>1596.6410085084913</v>
+      </c>
+      <c r="CQ35">
+        <v>32</v>
+      </c>
+      <c r="CR35">
+        <v>1603.4016001699499</v>
+      </c>
+      <c r="CS35">
+        <v>3.8094047726704397E-2</v>
+      </c>
+      <c r="CT35">
+        <v>0.31582058759958898</v>
+      </c>
+      <c r="CU35">
+        <v>1</v>
+      </c>
+      <c r="CV35">
+        <v>0</v>
+      </c>
+      <c r="CW35">
+        <f t="shared" si="19"/>
+        <v>1611.6893699541226</v>
+      </c>
     </row>
-    <row r="36" spans="1:83">
+    <row r="36" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>33</v>
       </c>
@@ -9112,6 +11098,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG36">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH36">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI36">
         <v>33</v>
       </c>
@@ -9137,7 +11131,7 @@
         <v>3.4083011176298701E-2</v>
       </c>
       <c r="AQ36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>740.16590880638034</v>
       </c>
       <c r="AS36">
@@ -9193,15 +11187,15 @@
         <v>4.3191799999999997E-3</v>
       </c>
       <c r="BL36">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>722.73946357142859</v>
       </c>
       <c r="BN36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO36" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP36" s="3">
@@ -9223,7 +11217,7 @@
         <v>1.2911789999999999E-2</v>
       </c>
       <c r="BV36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>681.90521778417258</v>
       </c>
       <c r="BX36">
@@ -9248,11 +11242,61 @@
         <v>3.4768313405347299E-2</v>
       </c>
       <c r="CE36">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>678.39021431654464</v>
       </c>
+      <c r="CG36">
+        <v>33</v>
+      </c>
+      <c r="CH36">
+        <v>670.58433581587406</v>
+      </c>
+      <c r="CI36">
+        <v>8.4149937742762793E-3</v>
+      </c>
+      <c r="CJ36">
+        <v>0.47979918775500902</v>
+      </c>
+      <c r="CK36">
+        <v>0.93697693382360203</v>
+      </c>
+      <c r="CL36">
+        <v>1.14269808442167E-2</v>
+      </c>
+      <c r="CM36">
+        <v>1</v>
+      </c>
+      <c r="CN36">
+        <v>0</v>
+      </c>
+      <c r="CO36">
+        <f t="shared" si="18"/>
+        <v>683.19747450200543</v>
+      </c>
+      <c r="CQ36">
+        <v>33</v>
+      </c>
+      <c r="CR36">
+        <v>719.04397070366304</v>
+      </c>
+      <c r="CS36">
+        <v>0.46359728791766802</v>
+      </c>
+      <c r="CT36">
+        <v>0.25940115634646599</v>
+      </c>
+      <c r="CU36">
+        <v>1</v>
+      </c>
+      <c r="CV36">
+        <v>2.8452764244518099E-2</v>
+      </c>
+      <c r="CW36">
+        <f t="shared" si="19"/>
+        <v>727.33174048783565</v>
+      </c>
     </row>
-    <row r="37" spans="1:83" s="2" customFormat="1">
+    <row r="37" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>34</v>
       </c>
@@ -9350,6 +11394,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AG37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH37">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="AI37">
         <v>34</v>
       </c>
@@ -9375,7 +11427,7 @@
         <v>0</v>
       </c>
       <c r="AQ37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1271.3231934570713</v>
       </c>
       <c r="AS37">
@@ -9431,15 +11483,15 @@
         <v>3.5949790000000002E-2</v>
       </c>
       <c r="BL37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1194.6365585714286</v>
       </c>
       <c r="BN37">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO37" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP37" s="3">
@@ -9461,7 +11513,7 @@
         <v>1.75592E-3</v>
       </c>
       <c r="BV37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1192.5575197841727</v>
       </c>
       <c r="BX37">
@@ -9486,11 +11538,61 @@
         <v>0.63492130176112405</v>
       </c>
       <c r="CE37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1183.7664636665356</v>
       </c>
+      <c r="CG37">
+        <v>34</v>
+      </c>
+      <c r="CH37">
+        <v>1170.5599847538599</v>
+      </c>
+      <c r="CI37">
+        <v>2.44360877070742E-2</v>
+      </c>
+      <c r="CJ37">
+        <v>0.23692769184595799</v>
+      </c>
+      <c r="CK37">
+        <v>1</v>
+      </c>
+      <c r="CL37">
+        <v>3.1644501632790301E-3</v>
+      </c>
+      <c r="CM37">
+        <v>0.80487233891559296</v>
+      </c>
+      <c r="CN37">
+        <v>4.3473532485477197E-3</v>
+      </c>
+      <c r="CO37">
+        <f t="shared" si="18"/>
+        <v>1183.1731234399913</v>
+      </c>
+      <c r="CQ37">
+        <v>34</v>
+      </c>
+      <c r="CR37">
+        <v>1294.6347162418001</v>
+      </c>
+      <c r="CS37">
+        <v>0.27234024538467499</v>
+      </c>
+      <c r="CT37">
+        <v>0.16431605643106501</v>
+      </c>
+      <c r="CU37">
+        <v>1</v>
+      </c>
+      <c r="CV37">
+        <v>3.9654348553289399E-3</v>
+      </c>
+      <c r="CW37">
+        <f t="shared" si="19"/>
+        <v>1302.9224860259728</v>
+      </c>
     </row>
-    <row r="38" spans="1:83">
+    <row r="38" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>35</v>
       </c>
@@ -9572,7 +11674,7 @@
         <v>0</v>
       </c>
       <c r="AC38">
-        <f t="shared" si="6"/>
+        <f>IF(AND(G38&gt;Y38, N38&gt;Y38, Y38&lt;AQ38,Y38&lt;BC38, Y38&lt;CE38, Y38&lt;CO38, Y38&lt;CW38),1,0)</f>
         <v>0</v>
       </c>
       <c r="AD38">
@@ -9585,7 +11687,15 @@
       </c>
       <c r="AF38">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AG38">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AH38">
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
       <c r="AI38">
         <v>35</v>
@@ -9612,7 +11722,7 @@
         <v>0</v>
       </c>
       <c r="AQ38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>962.32666639540741</v>
       </c>
       <c r="AS38">
@@ -9668,15 +11778,15 @@
         <v>4.0234579999999999E-2</v>
       </c>
       <c r="BL38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>800.33718357142857</v>
       </c>
       <c r="BN38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BO38" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="BP38" s="3">
@@ -9698,7 +11808,7 @@
         <v>1.86797E-3</v>
       </c>
       <c r="BV38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>801.81272878417258</v>
       </c>
       <c r="BX38">
@@ -9723,11 +11833,61 @@
         <v>0.58478435831143805</v>
       </c>
       <c r="CE38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>753.41629646825766</v>
       </c>
+      <c r="CG38">
+        <v>35</v>
+      </c>
+      <c r="CH38">
+        <v>740.34333473594199</v>
+      </c>
+      <c r="CI38">
+        <v>4.5185434380067599E-2</v>
+      </c>
+      <c r="CJ38">
+        <v>0.24770663154134601</v>
+      </c>
+      <c r="CK38">
+        <v>1</v>
+      </c>
+      <c r="CL38">
+        <v>6.8108542713621496E-3</v>
+      </c>
+      <c r="CM38">
+        <v>0.50983415191844506</v>
+      </c>
+      <c r="CN38">
+        <v>0</v>
+      </c>
+      <c r="CO38">
+        <f t="shared" si="18"/>
+        <v>752.95647342207337</v>
+      </c>
+      <c r="CQ38">
+        <v>35</v>
+      </c>
+      <c r="CR38">
+        <v>783.50985092670396</v>
+      </c>
+      <c r="CS38">
+        <v>0.68746857466716504</v>
+      </c>
+      <c r="CT38">
+        <v>0.22873952529434499</v>
+      </c>
+      <c r="CU38">
+        <v>1</v>
+      </c>
+      <c r="CV38">
+        <v>1.44511479871551E-2</v>
+      </c>
+      <c r="CW38">
+        <f t="shared" si="19"/>
+        <v>791.79762071087657</v>
+      </c>
     </row>
-    <row r="39" spans="1:83">
+    <row r="39" spans="1:101" x14ac:dyDescent="0.2">
       <c r="F39">
         <f>AVERAGE(F3:F38)</f>
         <v>7.4534027524388686E-3</v>
@@ -9746,27 +11906,35 @@
       </c>
       <c r="AA39">
         <f>SUM(AA3:AA38)</f>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="AB39">
-        <f t="shared" ref="AB39:AF39" si="16">SUM(AB3:AB38)</f>
+        <f t="shared" ref="AB39:AH39" si="20">SUM(AB3:AB38)</f>
         <v>0</v>
       </c>
       <c r="AC39">
-        <f t="shared" si="16"/>
-        <v>1</v>
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
       <c r="AD39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AE39">
-        <f t="shared" si="16"/>
-        <v>16</v>
+        <f t="shared" si="20"/>
+        <v>14</v>
       </c>
       <c r="AF39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
+        <v>5</v>
+      </c>
+      <c r="AG39">
+        <f t="shared" si="20"/>
         <v>6</v>
+      </c>
+      <c r="AH39">
+        <f t="shared" si="20"/>
+        <v>2</v>
       </c>
       <c r="AQ39">
         <f>SUM(AQ3:AQ38)</f>
@@ -9788,8 +11956,16 @@
         <f>SUM(CE3:CE38)</f>
         <v>38294.183241427789</v>
       </c>
+      <c r="CO39">
+        <f>SUM(CO3:CO38)</f>
+        <v>38350.774126374112</v>
+      </c>
+      <c r="CW39">
+        <f>SUM(CW3:CW38)</f>
+        <v>40507.282365096406</v>
+      </c>
     </row>
-    <row r="40" spans="1:83">
+    <row r="40" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -9813,8 +11989,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="BP3:BU38">
-    <sortCondition ref="BP2"/>
+  <sortState ref="CQ3:CV38">
+    <sortCondition ref="CQ2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
MF attention new fit result
</commit_message>
<xml_diff>
--- a/data_analysis/fit_result.xlsx
+++ b/data_analysis/fit_result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zac/Documents/RLpsy/data_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Developer/Python/RLpsy/data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9D7B4272-1E3A-6F4A-90F3-14100F4B9578}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{522A743A-60C5-9345-A170-F6603800539E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14160" yWindow="12600" windowWidth="44260" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="24760" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MF_fit_result" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="26">
   <si>
     <t>participant</t>
   </si>
@@ -94,9 +94,6 @@
     <t>alpha_attention</t>
   </si>
   <si>
-    <t>forget_attention</t>
-  </si>
-  <si>
     <t>MF_attention</t>
   </si>
   <si>
@@ -107,7 +104,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -954,16 +951,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CW40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O13" workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3:AH38"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AE20" sqref="AE20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:101">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -989,13 +988,13 @@
         <v>21</v>
       </c>
       <c r="CG1" t="s">
+        <v>24</v>
+      </c>
+      <c r="CQ1" t="s">
         <v>25</v>
       </c>
-      <c r="CQ1" t="s">
-        <v>26</v>
-      </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:101">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1084,10 +1083,10 @@
         <v>22</v>
       </c>
       <c r="AG2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH2" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="AI2" t="s">
         <v>0</v>
@@ -1236,9 +1235,6 @@
       <c r="CM2" t="s">
         <v>23</v>
       </c>
-      <c r="CN2" t="s">
-        <v>24</v>
-      </c>
       <c r="CO2" t="s">
         <v>11</v>
       </c>
@@ -1264,7 +1260,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:101">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1355,7 +1351,7 @@
       </c>
       <c r="AE3">
         <f>IF(AND(G3&gt;BC3, Y3&gt;BC3, G3&gt;BC3,AQ3&gt;BC3,BC3&lt;CE3, BC3&lt;CO3, BC3&lt;CW3),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF3">
         <f>IF(AND(G3&gt;CE3, Y3&gt;CE3, N3&gt;CE3,AQ3&gt;CE3,BC3&gt;CE3, CE3&lt;CO3, CE3&lt;CW3),1,0)</f>
@@ -1363,7 +1359,7 @@
       </c>
       <c r="AG3">
         <f>IF(AND(G3&gt;CO3, Y3&gt;CO3, N3&gt;CO3,AQ3&gt;CO3,BC3&gt;CO3, CE3&gt;CO3, CO3&lt;CW3),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH3">
         <f>IF(AND(G3&gt;CW3, Y3&gt;CW3, N3&gt;CW3,AQ3&gt;CW3,BC3&gt;CW3, CE3&gt;CW3, CO3&gt;CW3),1,0)</f>
@@ -1512,29 +1508,26 @@
         <v>0</v>
       </c>
       <c r="CH3">
-        <v>948.51045369062399</v>
+        <v>947.23047099185999</v>
       </c>
       <c r="CI3">
-        <v>3.8915330706178003E-2</v>
+        <v>4.7894909786071603E-2</v>
       </c>
       <c r="CJ3">
-        <v>0.61371789523851705</v>
+        <v>0.61060513117372495</v>
       </c>
       <c r="CK3">
         <v>1</v>
       </c>
       <c r="CL3">
-        <v>2.6934781151845598E-3</v>
+        <v>2.1005000749185899E-3</v>
       </c>
       <c r="CM3">
-        <v>1.2043779259776E-2</v>
-      </c>
-      <c r="CN3">
-        <v>0</v>
+        <v>3.2704855949165701E-3</v>
       </c>
       <c r="CO3">
-        <f>CH3+2*6*(144/(144-6-1))</f>
-        <v>961.12359237675537</v>
+        <f>CH3+2*5*(144/(144-5-1))</f>
+        <v>957.66525360055562</v>
       </c>
       <c r="CQ3">
         <v>0</v>
@@ -1559,7 +1552,7 @@
         <v>1070.4097376210327</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:101">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1807,29 +1800,26 @@
         <v>1</v>
       </c>
       <c r="CH4">
-        <v>1635.34725024046</v>
+        <v>1633.3692285536399</v>
       </c>
       <c r="CI4">
-        <v>1.3543457546678401E-2</v>
+        <v>1.29945970923526E-2</v>
       </c>
       <c r="CJ4">
-        <v>0.16495681426310399</v>
+        <v>0.20616195662891801</v>
       </c>
       <c r="CK4">
         <v>1</v>
       </c>
-      <c r="CL4" s="1">
-        <v>9.5044858105273504E-5</v>
+      <c r="CL4">
+        <v>0</v>
       </c>
       <c r="CM4">
-        <v>0.96517727550497001</v>
-      </c>
-      <c r="CN4">
-        <v>1.9502928637971199E-3</v>
+        <v>0.11405463407296</v>
       </c>
       <c r="CO4">
-        <f t="shared" ref="CO4:CO38" si="18">CH4+2*6*(144/(144-6-1))</f>
-        <v>1647.9603889265913</v>
+        <f t="shared" ref="CO4:CO38" si="18">CH4+2*5*(144/(144-5-1))</f>
+        <v>1643.8040111623357</v>
       </c>
       <c r="CQ4">
         <v>1</v>
@@ -1854,7 +1844,7 @@
         <v>1668.7708517711328</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:101">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2102,29 +2092,26 @@
         <v>2</v>
       </c>
       <c r="CH5">
-        <v>1494.5970165056499</v>
+        <v>1493.6195121759499</v>
       </c>
       <c r="CI5">
-        <v>2.0496989743865001E-2</v>
+        <v>2.98128816389625E-2</v>
       </c>
       <c r="CJ5">
-        <v>0.24548109779379601</v>
+        <v>0.20652189228565601</v>
       </c>
       <c r="CK5">
         <v>1</v>
       </c>
       <c r="CL5">
-        <v>7.2306813513348003E-4</v>
+        <v>1.8243993068673501E-3</v>
       </c>
       <c r="CM5">
-        <v>0.29469265805834999</v>
-      </c>
-      <c r="CN5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CO5">
         <f t="shared" si="18"/>
-        <v>1507.2101551917813</v>
+        <v>1504.0542947846457</v>
       </c>
       <c r="CQ5">
         <v>2</v>
@@ -2149,7 +2136,7 @@
         <v>1441.4431506675028</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:101">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2240,7 +2227,7 @@
       </c>
       <c r="AE6">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6">
         <f t="shared" si="9"/>
@@ -2248,7 +2235,7 @@
       </c>
       <c r="AG6">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6">
         <f t="shared" si="11"/>
@@ -2397,29 +2384,26 @@
         <v>3</v>
       </c>
       <c r="CH6">
-        <v>648.17146157898298</v>
+        <v>640.80478269047103</v>
       </c>
       <c r="CI6">
-        <v>2.8629892594353099E-2</v>
+        <v>2.4904003240265499E-2</v>
       </c>
       <c r="CJ6">
-        <v>0.43562658565628898</v>
+        <v>0.81601211396102402</v>
       </c>
       <c r="CK6">
         <v>1</v>
       </c>
       <c r="CL6">
-        <v>3.4945006712880797E-2</v>
+        <v>0.05</v>
       </c>
       <c r="CM6">
-        <v>0.20176045508447599</v>
-      </c>
-      <c r="CN6">
-        <v>4.36666381297915E-4</v>
+        <v>3.5873554970198299E-2</v>
       </c>
       <c r="CO6">
         <f t="shared" si="18"/>
-        <v>660.78460026511436</v>
+        <v>651.23956529916666</v>
       </c>
       <c r="CQ6">
         <v>3</v>
@@ -2444,7 +2428,7 @@
         <v>681.80532136841362</v>
       </c>
     </row>
-    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:101">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2692,29 +2676,26 @@
         <v>4</v>
       </c>
       <c r="CH7">
-        <v>1923.3650736054201</v>
+        <v>1923.4562765736</v>
       </c>
       <c r="CI7">
-        <v>7.9874754835646294E-2</v>
+        <v>5.2709191587230399E-2</v>
       </c>
       <c r="CJ7">
-        <v>3.6145101110742699E-2</v>
+        <v>4.65101310121665E-2</v>
       </c>
       <c r="CK7">
-        <v>0.99981802729856695</v>
+        <v>1</v>
       </c>
       <c r="CL7">
-        <v>1.20055240746218E-3</v>
+        <v>1.22264857928721E-3</v>
       </c>
       <c r="CM7">
-        <v>1</v>
-      </c>
-      <c r="CN7">
-        <v>5.7307374299933799E-3</v>
+        <v>0.73735174440477003</v>
       </c>
       <c r="CO7">
         <f t="shared" si="18"/>
-        <v>1935.9782122915515</v>
+        <v>1933.8910591822957</v>
       </c>
       <c r="CQ7">
         <v>4</v>
@@ -2739,7 +2720,7 @@
         <v>1926.4685397870128</v>
       </c>
     </row>
-    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:101">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2987,29 +2968,26 @@
         <v>5</v>
       </c>
       <c r="CH8">
-        <v>788.81392239227898</v>
+        <v>784.95645056097999</v>
       </c>
       <c r="CI8">
-        <v>2.5019400000391399E-2</v>
+        <v>2.51021495502693E-2</v>
       </c>
       <c r="CJ8">
-        <v>0.30163260384053597</v>
+        <v>0.31619931157437597</v>
       </c>
       <c r="CK8">
         <v>1</v>
       </c>
       <c r="CL8">
-        <v>8.9595282752376205E-3</v>
+        <v>8.4045002950310106E-3</v>
       </c>
       <c r="CM8">
-        <v>0.69716875170043302</v>
-      </c>
-      <c r="CN8">
-        <v>0</v>
+        <v>0.205311174887297</v>
       </c>
       <c r="CO8">
         <f t="shared" si="18"/>
-        <v>801.42706107841036</v>
+        <v>795.39123316967562</v>
       </c>
       <c r="CQ8">
         <v>5</v>
@@ -3034,7 +3012,7 @@
         <v>864.62326212278958</v>
       </c>
     </row>
-    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:101">
       <c r="A9">
         <v>6</v>
       </c>
@@ -3282,29 +3260,26 @@
         <v>6</v>
       </c>
       <c r="CH9">
-        <v>1045.2269719532001</v>
+        <v>1048.3724388271401</v>
       </c>
       <c r="CI9">
-        <v>1.5659712809123299E-2</v>
+        <v>1.5827913691224101E-2</v>
       </c>
       <c r="CJ9">
-        <v>0.22480743457302199</v>
+        <v>0.228505306976791</v>
       </c>
       <c r="CK9">
         <v>1</v>
       </c>
       <c r="CL9">
-        <v>1.14099106972547E-3</v>
+        <v>1.3114041907544801E-3</v>
       </c>
       <c r="CM9">
-        <v>0.320237075842423</v>
-      </c>
-      <c r="CN9">
-        <v>0</v>
+        <v>0.167821559112807</v>
       </c>
       <c r="CO9">
         <f t="shared" si="18"/>
-        <v>1057.8401106393314</v>
+        <v>1058.8072214358358</v>
       </c>
       <c r="CQ9">
         <v>6</v>
@@ -3329,7 +3304,7 @@
         <v>1148.5445545715227</v>
       </c>
     </row>
-    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:101">
       <c r="A10">
         <v>7</v>
       </c>
@@ -3577,29 +3552,26 @@
         <v>7</v>
       </c>
       <c r="CH10">
-        <v>1220.00105430435</v>
+        <v>1207.0962398397201</v>
       </c>
       <c r="CI10">
-        <v>3.9866628676283801E-2</v>
+        <v>4.81774771221039E-2</v>
       </c>
       <c r="CJ10">
-        <v>0.29830240084623399</v>
+        <v>0.31181745353421297</v>
       </c>
       <c r="CK10">
         <v>1</v>
       </c>
       <c r="CL10">
-        <v>5.9650327839560601E-3</v>
+        <v>6.68339698135319E-3</v>
       </c>
       <c r="CM10">
-        <v>0.61219857696830604</v>
-      </c>
-      <c r="CN10">
-        <v>0</v>
+        <v>8.8639587226110997E-2</v>
       </c>
       <c r="CO10">
         <f t="shared" si="18"/>
-        <v>1232.6141929904813</v>
+        <v>1217.5310224484158</v>
       </c>
       <c r="CQ10">
         <v>7</v>
@@ -3624,7 +3596,7 @@
         <v>1243.3531431125227</v>
       </c>
     </row>
-    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:101">
       <c r="A11">
         <v>8</v>
       </c>
@@ -3715,7 +3687,7 @@
       </c>
       <c r="AE11">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF11">
         <f t="shared" si="9"/>
@@ -3723,7 +3695,7 @@
       </c>
       <c r="AG11">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH11">
         <f t="shared" si="11"/>
@@ -3872,29 +3844,26 @@
         <v>8</v>
       </c>
       <c r="CH11">
-        <v>921.48093901155903</v>
+        <v>925.10579459283804</v>
       </c>
       <c r="CI11">
-        <v>3.2654036668424202E-2</v>
+        <v>3.3119038499137797E-2</v>
       </c>
       <c r="CJ11">
-        <v>0.29078208985172999</v>
+        <v>0.30253494682714099</v>
       </c>
       <c r="CK11">
         <v>1</v>
       </c>
       <c r="CL11">
-        <v>1.74823100310799E-3</v>
+        <v>1.52351904441756E-3</v>
       </c>
       <c r="CM11">
-        <v>1</v>
-      </c>
-      <c r="CN11">
-        <v>0</v>
+        <v>0.76969410820804496</v>
       </c>
       <c r="CO11">
         <f t="shared" si="18"/>
-        <v>934.09407769769041</v>
+        <v>935.54057720153367</v>
       </c>
       <c r="CQ11">
         <v>8</v>
@@ -3919,7 +3888,7 @@
         <v>956.98012620138161</v>
       </c>
     </row>
-    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:101">
       <c r="A12">
         <v>9</v>
       </c>
@@ -4167,29 +4136,26 @@
         <v>9</v>
       </c>
       <c r="CH12">
-        <v>383.79313286458199</v>
+        <v>383.529276539232</v>
       </c>
       <c r="CI12">
-        <v>3.1408564879711103E-2</v>
+        <v>3.6485444909522199E-2</v>
       </c>
       <c r="CJ12">
-        <v>0.40904391050377398</v>
+        <v>0.41417997389150801</v>
       </c>
       <c r="CK12">
         <v>1</v>
       </c>
       <c r="CL12">
-        <v>8.2773107594032794E-3</v>
+        <v>9.4057402482840193E-3</v>
       </c>
       <c r="CM12">
-        <v>1</v>
-      </c>
-      <c r="CN12">
-        <v>0</v>
+        <v>0.55285666567956604</v>
       </c>
       <c r="CO12">
         <f t="shared" si="18"/>
-        <v>396.40627155071337</v>
+        <v>393.96405914792763</v>
       </c>
       <c r="CQ12">
         <v>9</v>
@@ -4214,7 +4180,7 @@
         <v>518.9928784746777</v>
       </c>
     </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:101">
       <c r="A13">
         <v>10</v>
       </c>
@@ -4462,29 +4428,26 @@
         <v>10</v>
       </c>
       <c r="CH13">
-        <v>933.75653020790799</v>
+        <v>940.00846271801095</v>
       </c>
       <c r="CI13">
-        <v>2.54070464572499E-2</v>
+        <v>2.5388464497563299E-2</v>
       </c>
       <c r="CJ13">
-        <v>0.276736408280982</v>
+        <v>0.27742123835669003</v>
       </c>
       <c r="CK13">
         <v>1</v>
       </c>
       <c r="CL13">
-        <v>5.4381711406875002E-3</v>
+        <v>5.92447108905228E-3</v>
       </c>
       <c r="CM13">
-        <v>0.97542871234347495</v>
-      </c>
-      <c r="CN13">
-        <v>0</v>
+        <v>0.877262169941599</v>
       </c>
       <c r="CO13">
         <f t="shared" si="18"/>
-        <v>946.36966889403936</v>
+        <v>950.44324532670657</v>
       </c>
       <c r="CQ13">
         <v>10</v>
@@ -4509,7 +4472,7 @@
         <v>1038.6963621769528</v>
       </c>
     </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:101">
       <c r="A14">
         <v>11</v>
       </c>
@@ -4600,7 +4563,7 @@
       </c>
       <c r="AE14">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF14">
         <f t="shared" si="9"/>
@@ -4608,7 +4571,7 @@
       </c>
       <c r="AG14">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH14">
         <f t="shared" si="11"/>
@@ -4757,29 +4720,26 @@
         <v>11</v>
       </c>
       <c r="CH14">
-        <v>861.04034754566703</v>
+        <v>843.68119463619098</v>
       </c>
       <c r="CI14">
-        <v>1.8494963590483401E-2</v>
+        <v>2.4218331828760702E-2</v>
       </c>
       <c r="CJ14">
-        <v>0.334839693100281</v>
+        <v>0.40228563619151703</v>
       </c>
       <c r="CK14">
         <v>1</v>
       </c>
       <c r="CL14">
-        <v>2.4809448412138799E-3</v>
+        <v>2.807595019862E-3</v>
       </c>
       <c r="CM14">
-        <v>0.22971138660778001</v>
-      </c>
-      <c r="CN14">
-        <v>0</v>
+        <v>2.75777796249967E-2</v>
       </c>
       <c r="CO14">
         <f t="shared" si="18"/>
-        <v>873.65348623179841</v>
+        <v>854.11597724488661</v>
       </c>
       <c r="CQ14">
         <v>11</v>
@@ -4804,7 +4764,7 @@
         <v>926.74580304951962</v>
       </c>
     </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:101">
       <c r="A15">
         <v>12</v>
       </c>
@@ -4879,7 +4839,7 @@
       </c>
       <c r="AA15">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB15">
         <f t="shared" si="5"/>
@@ -4903,7 +4863,7 @@
       </c>
       <c r="AG15">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH15">
         <f t="shared" si="11"/>
@@ -5052,29 +5012,26 @@
         <v>12</v>
       </c>
       <c r="CH15">
-        <v>689.09298749609502</v>
+        <v>686.85547312950405</v>
       </c>
       <c r="CI15">
-        <v>1.6746507269712E-2</v>
+        <v>2.2259312604702399E-2</v>
       </c>
       <c r="CJ15">
-        <v>0.28394282968711199</v>
+        <v>0.31460296697367301</v>
       </c>
       <c r="CK15">
         <v>1</v>
       </c>
       <c r="CL15">
-        <v>4.3531140389501304E-3</v>
+        <v>5.9929900014293004E-3</v>
       </c>
       <c r="CM15">
-        <v>0.97721014855647004</v>
-      </c>
-      <c r="CN15">
-        <v>0</v>
+        <v>0.17772417219157499</v>
       </c>
       <c r="CO15">
         <f t="shared" si="18"/>
-        <v>701.7061261822264</v>
+        <v>697.29025573819968</v>
       </c>
       <c r="CQ15">
         <v>12</v>
@@ -5099,7 +5056,7 @@
         <v>875.48054281374357</v>
       </c>
     </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:101">
       <c r="A16">
         <v>13</v>
       </c>
@@ -5347,29 +5304,26 @@
         <v>13</v>
       </c>
       <c r="CH16">
-        <v>902.22344282769097</v>
+        <v>904.86941138178395</v>
       </c>
       <c r="CI16">
-        <v>2.9448745826485601E-2</v>
+        <v>2.4590692859245099E-2</v>
       </c>
       <c r="CJ16">
-        <v>0.33625213426407302</v>
+        <v>0.39253478787592799</v>
       </c>
       <c r="CK16">
         <v>1</v>
       </c>
       <c r="CL16">
-        <v>2.65451519594571E-2</v>
+        <v>2.9201555757163999E-2</v>
       </c>
       <c r="CM16">
-        <v>0.27285516809436899</v>
-      </c>
-      <c r="CN16">
-        <v>0</v>
+        <v>7.7011019550151202E-2</v>
       </c>
       <c r="CO16">
         <f t="shared" si="18"/>
-        <v>914.83658151382235</v>
+        <v>915.30419399047958</v>
       </c>
       <c r="CQ16">
         <v>13</v>
@@ -5394,7 +5348,7 @@
         <v>937.21743143530864</v>
       </c>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:101">
       <c r="A17">
         <v>14</v>
       </c>
@@ -5642,29 +5596,26 @@
         <v>14</v>
       </c>
       <c r="CH17">
-        <v>1591.1071221636801</v>
+        <v>1591.48186549099</v>
       </c>
       <c r="CI17">
-        <v>5.0239171900815602E-2</v>
+        <v>3.9991087917080503E-2</v>
       </c>
       <c r="CJ17">
-        <v>0.28006468287201602</v>
+        <v>0.30531698231731702</v>
       </c>
       <c r="CK17">
         <v>1</v>
       </c>
       <c r="CL17">
-        <v>1.0417966530518201E-3</v>
+        <v>1.7946631758002801E-3</v>
       </c>
       <c r="CM17">
-        <v>0.48858925521928198</v>
-      </c>
-      <c r="CN17">
-        <v>3.3933558986764499E-3</v>
+        <v>0.66969523376502105</v>
       </c>
       <c r="CO17">
         <f t="shared" si="18"/>
-        <v>1603.7202608498114</v>
+        <v>1601.9166480996857</v>
       </c>
       <c r="CQ17">
         <v>14</v>
@@ -5689,7 +5640,7 @@
         <v>1629.9795576430727</v>
       </c>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:101">
       <c r="A18">
         <v>15</v>
       </c>
@@ -5937,29 +5888,26 @@
         <v>15</v>
       </c>
       <c r="CH18">
-        <v>1331.32397729493</v>
+        <v>1329.45431144281</v>
       </c>
       <c r="CI18">
-        <v>3.8192921771887899E-2</v>
+        <v>4.4982202285592097E-2</v>
       </c>
       <c r="CJ18">
-        <v>0.25305423498319601</v>
+        <v>0.27853997886564702</v>
       </c>
       <c r="CK18">
         <v>1</v>
       </c>
       <c r="CL18">
-        <v>6.6739298723252696E-3</v>
+        <v>1.32083332266635E-2</v>
       </c>
       <c r="CM18">
-        <v>0.36908079349563899</v>
-      </c>
-      <c r="CN18">
-        <v>0</v>
+        <v>8.2212173270953995E-2</v>
       </c>
       <c r="CO18">
         <f t="shared" si="18"/>
-        <v>1343.9371159810614</v>
+        <v>1339.8890940515057</v>
       </c>
       <c r="CQ18">
         <v>15</v>
@@ -5984,7 +5932,7 @@
         <v>1374.7685146442427</v>
       </c>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:101">
       <c r="A19">
         <v>16</v>
       </c>
@@ -6067,7 +6015,7 @@
       </c>
       <c r="AC19">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD19">
         <f t="shared" si="7"/>
@@ -6083,7 +6031,7 @@
       </c>
       <c r="AG19">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH19">
         <f t="shared" si="11"/>
@@ -6232,29 +6180,26 @@
         <v>16</v>
       </c>
       <c r="CH19">
-        <v>438.43470471005497</v>
+        <v>443.96091294596698</v>
       </c>
       <c r="CI19">
-        <v>1.8466122887919802E-2</v>
+        <v>1.39700477798757E-2</v>
       </c>
       <c r="CJ19">
-        <v>0.41299104747947402</v>
+        <v>0.41939491990778499</v>
       </c>
       <c r="CK19">
         <v>1</v>
       </c>
       <c r="CL19">
-        <v>3.4039133178603901E-3</v>
+        <v>2.9019237886204301E-3</v>
       </c>
       <c r="CM19">
-        <v>0.356597147034732</v>
-      </c>
-      <c r="CN19">
-        <v>0</v>
+        <v>0.67660706456995701</v>
       </c>
       <c r="CO19">
         <f t="shared" si="18"/>
-        <v>451.04784339618635</v>
+        <v>454.39569555466261</v>
       </c>
       <c r="CQ19">
         <v>16</v>
@@ -6279,7 +6224,7 @@
         <v>710.19755523265758</v>
       </c>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:101">
       <c r="A20">
         <v>17</v>
       </c>
@@ -6527,29 +6472,26 @@
         <v>17</v>
       </c>
       <c r="CH20">
-        <v>1008.15989311806</v>
+        <v>1003.4106678437701</v>
       </c>
       <c r="CI20">
-        <v>2.0265967685290001E-2</v>
+        <v>2.8371171340926201E-2</v>
       </c>
       <c r="CJ20">
-        <v>0.25159358755327599</v>
+        <v>0.29006359927590197</v>
       </c>
       <c r="CK20">
         <v>1</v>
       </c>
       <c r="CL20">
-        <v>8.6966823885079904E-3</v>
+        <v>8.5347673168482806E-3</v>
       </c>
       <c r="CM20">
-        <v>1</v>
-      </c>
-      <c r="CN20">
-        <v>0</v>
+        <v>5.1714001577231598E-2</v>
       </c>
       <c r="CO20">
         <f t="shared" si="18"/>
-        <v>1020.7730318041914</v>
+        <v>1013.8454504524657</v>
       </c>
       <c r="CQ20">
         <v>17</v>
@@ -6574,7 +6516,7 @@
         <v>1071.8021693203827</v>
       </c>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:101">
       <c r="A21">
         <v>18</v>
       </c>
@@ -6822,29 +6764,26 @@
         <v>18</v>
       </c>
       <c r="CH21">
-        <v>1882.16499760478</v>
+        <v>1892.55708582335</v>
       </c>
       <c r="CI21">
-        <v>2.0932613816704401E-2</v>
+        <v>0.110070757269657</v>
       </c>
       <c r="CJ21">
-        <v>0.10693473226174</v>
+        <v>5.30142085743497E-2</v>
       </c>
       <c r="CK21">
         <v>1</v>
       </c>
       <c r="CL21">
-        <v>3.0573594975778101E-4</v>
+        <v>6.6763516156531002E-3</v>
       </c>
       <c r="CM21">
-        <v>1</v>
-      </c>
-      <c r="CN21">
-        <v>7.1414480001892101E-4</v>
+        <v>0.99121708601144198</v>
       </c>
       <c r="CO21">
         <f t="shared" si="18"/>
-        <v>1894.7781362909113</v>
+        <v>1902.9918684320457</v>
       </c>
       <c r="CQ21">
         <v>18</v>
@@ -6869,7 +6808,7 @@
         <v>1900.3364923509528</v>
       </c>
     </row>
-    <row r="22" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:101">
       <c r="A22">
         <v>19</v>
       </c>
@@ -7117,29 +7056,26 @@
         <v>19</v>
       </c>
       <c r="CH22">
-        <v>497.47147806294203</v>
+        <v>496.13112555831299</v>
       </c>
       <c r="CI22">
-        <v>3.0633438504594299E-2</v>
+        <v>2.52313511638338E-2</v>
       </c>
       <c r="CJ22">
-        <v>0.298661091911604</v>
+        <v>0.30803651916283198</v>
       </c>
       <c r="CK22">
         <v>1</v>
       </c>
       <c r="CL22">
-        <v>8.8990782351395705E-3</v>
+        <v>7.9092130323601302E-3</v>
       </c>
       <c r="CM22">
-        <v>0.85096622266147304</v>
-      </c>
-      <c r="CN22">
-        <v>2.1019294833146698E-2</v>
+        <v>0.859703671102239</v>
       </c>
       <c r="CO22">
         <f t="shared" si="18"/>
-        <v>510.0846167490734</v>
+        <v>506.56590816700862</v>
       </c>
       <c r="CQ22">
         <v>19</v>
@@ -7164,7 +7100,7 @@
         <v>559.34170146737961</v>
       </c>
     </row>
-    <row r="23" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:101" s="2" customFormat="1">
       <c r="A23">
         <v>20</v>
       </c>
@@ -7413,29 +7349,27 @@
         <v>20</v>
       </c>
       <c r="CH23">
-        <v>1107.3393843762799</v>
+        <v>1109.8436367035899</v>
       </c>
       <c r="CI23">
-        <v>1.6553006870076999E-2</v>
+        <v>1.7044396993411499E-2</v>
       </c>
       <c r="CJ23">
-        <v>0.271640826376078</v>
+        <v>0.27301164392362598</v>
       </c>
       <c r="CK23">
         <v>1</v>
       </c>
       <c r="CL23">
-        <v>0</v>
+        <v>1.65924409022183E-4</v>
       </c>
       <c r="CM23">
-        <v>9.7700540025135493E-2</v>
-      </c>
-      <c r="CN23">
-        <v>0</v>
-      </c>
+        <v>3.7573756762696801E-2</v>
+      </c>
+      <c r="CN23"/>
       <c r="CO23">
         <f t="shared" si="18"/>
-        <v>1119.9525230624113</v>
+        <v>1120.2784193122857</v>
       </c>
       <c r="CQ23">
         <v>20</v>
@@ -7460,7 +7394,7 @@
         <v>1242.8064529384528</v>
       </c>
     </row>
-    <row r="24" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:101">
       <c r="A24">
         <v>21</v>
       </c>
@@ -7535,7 +7469,7 @@
       </c>
       <c r="AA24">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB24">
         <f t="shared" si="5"/>
@@ -7559,7 +7493,7 @@
       </c>
       <c r="AG24">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH24">
         <f t="shared" si="11"/>
@@ -7708,29 +7642,26 @@
         <v>21</v>
       </c>
       <c r="CH24">
-        <v>1066.93244473963</v>
+        <v>1065.30366649603</v>
       </c>
       <c r="CI24">
-        <v>3.5890293364817902E-2</v>
+        <v>3.0822161267924999E-2</v>
       </c>
       <c r="CJ24">
-        <v>0.22923193329069799</v>
+        <v>0.23986388216361099</v>
       </c>
       <c r="CK24">
         <v>1</v>
       </c>
       <c r="CL24">
-        <v>7.8882163928771492E-3</v>
+        <v>7.54703573865318E-3</v>
       </c>
       <c r="CM24">
-        <v>0.17784209899878001</v>
-      </c>
-      <c r="CN24">
-        <v>0</v>
+        <v>0.11487229362068301</v>
       </c>
       <c r="CO24">
         <f t="shared" si="18"/>
-        <v>1079.5455834257614</v>
+        <v>1075.7384491047258</v>
       </c>
       <c r="CQ24">
         <v>21</v>
@@ -7755,7 +7686,7 @@
         <v>1095.9206739409028</v>
       </c>
     </row>
-    <row r="25" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:101">
       <c r="A25">
         <v>22</v>
       </c>
@@ -7830,7 +7761,7 @@
       </c>
       <c r="AA25">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB25">
         <f t="shared" si="5"/>
@@ -7854,7 +7785,7 @@
       </c>
       <c r="AG25">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH25">
         <f t="shared" si="11"/>
@@ -8003,29 +7934,26 @@
         <v>22</v>
       </c>
       <c r="CH25">
-        <v>898.18630950090096</v>
+        <v>897.65266997752997</v>
       </c>
       <c r="CI25">
-        <v>2.3838747170836502E-2</v>
+        <v>2.2841971768330901E-2</v>
       </c>
       <c r="CJ25">
-        <v>0.24306922043211199</v>
+        <v>0.25077424398370701</v>
       </c>
       <c r="CK25">
         <v>1</v>
       </c>
       <c r="CL25">
-        <v>4.2863317482380097E-3</v>
+        <v>4.6177416471065904E-3</v>
       </c>
       <c r="CM25">
-        <v>0.204608611766946</v>
-      </c>
-      <c r="CN25">
-        <v>0</v>
+        <v>0.100181559443678</v>
       </c>
       <c r="CO25">
         <f t="shared" si="18"/>
-        <v>910.79944818703234</v>
+        <v>908.0874525862256</v>
       </c>
       <c r="CQ25">
         <v>22</v>
@@ -8050,7 +7978,7 @@
         <v>1028.3694206605726</v>
       </c>
     </row>
-    <row r="26" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:101">
       <c r="A26">
         <v>23</v>
       </c>
@@ -8298,29 +8226,26 @@
         <v>23</v>
       </c>
       <c r="CH26">
-        <v>1043.8797422115199</v>
+        <v>1039.9884587086899</v>
       </c>
       <c r="CI26">
-        <v>2.1054859228923799E-2</v>
+        <v>2.52426327053718E-2</v>
       </c>
       <c r="CJ26">
-        <v>0.221530278625787</v>
+        <v>0.25262822483254299</v>
       </c>
       <c r="CK26">
         <v>1</v>
       </c>
       <c r="CL26">
-        <v>4.77130889976227E-3</v>
+        <v>5.4726485528365804E-3</v>
       </c>
       <c r="CM26">
-        <v>0.54758099829756601</v>
-      </c>
-      <c r="CN26">
-        <v>0</v>
+        <v>3.8793406093983497E-2</v>
       </c>
       <c r="CO26">
         <f t="shared" si="18"/>
-        <v>1056.4928808976513</v>
+        <v>1050.4232413173856</v>
       </c>
       <c r="CQ26">
         <v>23</v>
@@ -8345,7 +8270,7 @@
         <v>1078.9141639483528</v>
       </c>
     </row>
-    <row r="27" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:101">
       <c r="A27">
         <v>24</v>
       </c>
@@ -8593,29 +8518,26 @@
         <v>24</v>
       </c>
       <c r="CH27">
-        <v>940.66804231306401</v>
+        <v>945.31784817135599</v>
       </c>
       <c r="CI27">
-        <v>2.4351236192978899E-2</v>
+        <v>1.9873501647407602E-2</v>
       </c>
       <c r="CJ27">
-        <v>0.17176826643007301</v>
+        <v>0.193460669067578</v>
       </c>
       <c r="CK27">
-        <v>0.98899090941012402</v>
+        <v>0.899083749185418</v>
       </c>
       <c r="CL27">
-        <v>2.2530917268209498E-3</v>
+        <v>2.6075526965631101E-3</v>
       </c>
       <c r="CM27">
-        <v>0.77896862216699603</v>
-      </c>
-      <c r="CN27">
-        <v>3.5932512104094899E-2</v>
+        <v>0.83775583328182701</v>
       </c>
       <c r="CO27">
         <f t="shared" si="18"/>
-        <v>953.28118099919539</v>
+        <v>955.75263078005162</v>
       </c>
       <c r="CQ27">
         <v>24</v>
@@ -8640,7 +8562,7 @@
         <v>1013.1144915580226</v>
       </c>
     </row>
-    <row r="28" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:101">
       <c r="A28">
         <v>25</v>
       </c>
@@ -8731,7 +8653,7 @@
       </c>
       <c r="AE28">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF28">
         <f t="shared" si="9"/>
@@ -8739,7 +8661,7 @@
       </c>
       <c r="AG28">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH28">
         <f t="shared" si="11"/>
@@ -8888,29 +8810,26 @@
         <v>25</v>
       </c>
       <c r="CH28">
-        <v>749.38957869154297</v>
+        <v>750.55477410636797</v>
       </c>
       <c r="CI28">
-        <v>2.0107496773898399E-2</v>
+        <v>1.45054898283571E-2</v>
       </c>
       <c r="CJ28">
-        <v>0.43381782324523099</v>
+        <v>0.470835215982707</v>
       </c>
       <c r="CK28">
         <v>1</v>
       </c>
       <c r="CL28">
-        <v>1.48138842518087E-2</v>
+        <v>1.29698748648404E-2</v>
       </c>
       <c r="CM28">
-        <v>0.397999644476771</v>
-      </c>
-      <c r="CN28">
-        <v>3.1856140124859201E-3</v>
+        <v>0.373546634421696</v>
       </c>
       <c r="CO28">
         <f t="shared" si="18"/>
-        <v>762.00271737767434</v>
+        <v>760.9895567150636</v>
       </c>
       <c r="CQ28">
         <v>25</v>
@@ -8935,7 +8854,7 @@
         <v>816.10862977670263</v>
       </c>
     </row>
-    <row r="29" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:101" s="2" customFormat="1">
       <c r="A29">
         <v>26</v>
       </c>
@@ -9027,7 +8946,7 @@
       </c>
       <c r="AE29">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF29">
         <f t="shared" si="9"/>
@@ -9035,7 +8954,7 @@
       </c>
       <c r="AG29">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH29">
         <f t="shared" si="11"/>
@@ -9184,29 +9103,27 @@
         <v>26</v>
       </c>
       <c r="CH29">
-        <v>1807.0673928505</v>
+        <v>1813.06397875218</v>
       </c>
       <c r="CI29">
-        <v>4.05799857926184E-2</v>
+        <v>4.2279189467342999E-2</v>
       </c>
       <c r="CJ29">
-        <v>0.164023441985234</v>
+        <v>0.152995216602583</v>
       </c>
       <c r="CK29">
         <v>1</v>
       </c>
       <c r="CL29">
-        <v>2.2911498497076199E-3</v>
+        <v>2.3705941181769901E-3</v>
       </c>
       <c r="CM29">
-        <v>1</v>
-      </c>
-      <c r="CN29">
-        <v>0</v>
-      </c>
+        <v>0.97744644312976603</v>
+      </c>
+      <c r="CN29"/>
       <c r="CO29">
         <f t="shared" si="18"/>
-        <v>1819.6805315366314</v>
+        <v>1823.4987613608757</v>
       </c>
       <c r="CQ29">
         <v>26</v>
@@ -9231,7 +9148,7 @@
         <v>1875.6866412491327</v>
       </c>
     </row>
-    <row r="30" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:101">
       <c r="A30">
         <v>27</v>
       </c>
@@ -9479,29 +9396,26 @@
         <v>27</v>
       </c>
       <c r="CH30">
-        <v>691.84513330689003</v>
+        <v>693.15754956838498</v>
       </c>
       <c r="CI30">
-        <v>2.3877900888571699E-2</v>
+        <v>2.09251486238053E-2</v>
       </c>
       <c r="CJ30">
-        <v>0.34190364009580299</v>
+        <v>0.38127304158185799</v>
       </c>
       <c r="CK30">
         <v>1</v>
       </c>
       <c r="CL30">
-        <v>7.0612487290772604E-3</v>
+        <v>7.1885200186810397E-3</v>
       </c>
       <c r="CM30">
-        <v>1</v>
-      </c>
-      <c r="CN30">
-        <v>2.7526893459379299E-2</v>
+        <v>0.75685931511200299</v>
       </c>
       <c r="CO30">
         <f t="shared" si="18"/>
-        <v>704.45827199302141</v>
+        <v>703.59233217708061</v>
       </c>
       <c r="CQ30">
         <v>27</v>
@@ -9526,7 +9440,7 @@
         <v>780.51802711183063</v>
       </c>
     </row>
-    <row r="31" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:101">
       <c r="A31">
         <v>28</v>
       </c>
@@ -9601,7 +9515,7 @@
       </c>
       <c r="AA31">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB31">
         <f t="shared" si="5"/>
@@ -9625,7 +9539,7 @@
       </c>
       <c r="AG31">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH31">
         <f t="shared" si="11"/>
@@ -9774,29 +9688,26 @@
         <v>28</v>
       </c>
       <c r="CH31">
-        <v>783.03202907164496</v>
+        <v>780.73759402290705</v>
       </c>
       <c r="CI31">
-        <v>2.2067548673766198E-2</v>
+        <v>2.3025598758300202E-2</v>
       </c>
       <c r="CJ31">
-        <v>0.31834865634217602</v>
+        <v>0.31816729209344302</v>
       </c>
       <c r="CK31">
         <v>1</v>
       </c>
       <c r="CL31">
-        <v>3.72722668695894E-3</v>
+        <v>3.5660591904738701E-3</v>
       </c>
       <c r="CM31">
-        <v>0.46798819527413998</v>
-      </c>
-      <c r="CN31">
-        <v>0</v>
+        <v>0.23582587861739299</v>
       </c>
       <c r="CO31">
         <f t="shared" si="18"/>
-        <v>795.64516775777633</v>
+        <v>791.17237663160267</v>
       </c>
       <c r="CQ31">
         <v>28</v>
@@ -9821,7 +9732,7 @@
         <v>968.75915822313561</v>
       </c>
     </row>
-    <row r="32" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:101">
       <c r="A32">
         <v>29</v>
       </c>
@@ -10069,29 +9980,26 @@
         <v>29</v>
       </c>
       <c r="CH32">
-        <v>1258.1184197478999</v>
+        <v>1255.5762128984099</v>
       </c>
       <c r="CI32">
-        <v>0.26526501132694602</v>
+        <v>4.1162007226679301E-2</v>
       </c>
       <c r="CJ32">
-        <v>0.25037820557614199</v>
+        <v>0.30442158941948499</v>
       </c>
       <c r="CK32">
         <v>1</v>
       </c>
       <c r="CL32">
-        <v>1.7377154913007099E-2</v>
+        <v>3.7629321801288802E-3</v>
       </c>
       <c r="CM32">
-        <v>0.20837100700549999</v>
-      </c>
-      <c r="CN32">
-        <v>0</v>
+        <v>0.60225240750430398</v>
       </c>
       <c r="CO32">
         <f t="shared" si="18"/>
-        <v>1270.7315584340313</v>
+        <v>1266.0109955071057</v>
       </c>
       <c r="CQ32">
         <v>29</v>
@@ -10116,7 +10024,7 @@
         <v>1289.0662569749427</v>
       </c>
     </row>
-    <row r="33" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:101">
       <c r="A33">
         <v>30</v>
       </c>
@@ -10364,29 +10272,26 @@
         <v>30</v>
       </c>
       <c r="CH33">
-        <v>1341.89892354619</v>
+        <v>1337.5484041228301</v>
       </c>
       <c r="CI33">
-        <v>8.1816809503815299E-2</v>
+        <v>7.8353334033116201E-2</v>
       </c>
       <c r="CJ33">
-        <v>0.260690062958227</v>
+        <v>0.270002944995831</v>
       </c>
       <c r="CK33">
         <v>1</v>
       </c>
       <c r="CL33">
-        <v>3.14958916180957E-3</v>
+        <v>3.0909462263968498E-3</v>
       </c>
       <c r="CM33">
-        <v>4.2145041224265899E-2</v>
-      </c>
-      <c r="CN33">
-        <v>0</v>
+        <v>1.4287232166692899E-2</v>
       </c>
       <c r="CO33">
         <f t="shared" si="18"/>
-        <v>1354.5120622323213</v>
+        <v>1347.9831867315258</v>
       </c>
       <c r="CQ33">
         <v>30</v>
@@ -10411,7 +10316,7 @@
         <v>1365.1365519256328</v>
       </c>
     </row>
-    <row r="34" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:101">
       <c r="A34">
         <v>31</v>
       </c>
@@ -10659,29 +10564,26 @@
         <v>31</v>
       </c>
       <c r="CH34">
-        <v>898.74545101036199</v>
+        <v>900.81664418824403</v>
       </c>
       <c r="CI34">
-        <v>4.5553068810292599E-2</v>
+        <v>3.7140798163490599E-2</v>
       </c>
       <c r="CJ34">
-        <v>0.23596711247534</v>
+        <v>0.323386235929562</v>
       </c>
       <c r="CK34">
         <v>1</v>
       </c>
       <c r="CL34">
-        <v>5.6595216256657196E-3</v>
+        <v>8.4797742964255306E-3</v>
       </c>
       <c r="CM34">
-        <v>0.88230945686100903</v>
-      </c>
-      <c r="CN34">
-        <v>0.05</v>
+        <v>6.8570055357356399E-2</v>
       </c>
       <c r="CO34">
         <f t="shared" si="18"/>
-        <v>911.35858969649337</v>
+        <v>911.25142679693965</v>
       </c>
       <c r="CQ34">
         <v>31</v>
@@ -10706,7 +10608,7 @@
         <v>973.18298377771066</v>
       </c>
     </row>
-    <row r="35" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:101">
       <c r="A35">
         <v>32</v>
       </c>
@@ -10954,29 +10856,26 @@
         <v>32</v>
       </c>
       <c r="CH35">
-        <v>1584.0278698223599</v>
+        <v>1586.6275688102601</v>
       </c>
       <c r="CI35">
-        <v>0.99942042269162101</v>
+        <v>3.0273875284498901E-3</v>
       </c>
       <c r="CJ35">
-        <v>1.44922526426266</v>
+        <v>79.262377979588294</v>
       </c>
       <c r="CK35">
-        <v>0.99943630169832898</v>
+        <v>0</v>
       </c>
       <c r="CL35">
-        <v>4.10816422880013E-3</v>
+        <v>0</v>
       </c>
       <c r="CM35" s="1">
-        <v>5.8879053967172897E-5</v>
-      </c>
-      <c r="CN35">
-        <v>0</v>
+        <v>4.4973446679292903E-5</v>
       </c>
       <c r="CO35">
         <f t="shared" si="18"/>
-        <v>1596.6410085084913</v>
+        <v>1597.0623514189558</v>
       </c>
       <c r="CQ35">
         <v>32</v>
@@ -11001,7 +10900,7 @@
         <v>1611.6893699541226</v>
       </c>
     </row>
-    <row r="36" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:101">
       <c r="A36">
         <v>33</v>
       </c>
@@ -11249,29 +11148,26 @@
         <v>33</v>
       </c>
       <c r="CH36">
-        <v>670.58433581587406</v>
+        <v>670.15978069118705</v>
       </c>
       <c r="CI36">
-        <v>8.4149937742762793E-3</v>
+        <v>8.8736230650398509E-3</v>
       </c>
       <c r="CJ36">
-        <v>0.47979918775500902</v>
+        <v>0.45736049907190501</v>
       </c>
       <c r="CK36">
-        <v>0.93697693382360203</v>
+        <v>0.93277087613069098</v>
       </c>
       <c r="CL36">
-        <v>1.14269808442167E-2</v>
+        <v>1.10694019925257E-2</v>
       </c>
       <c r="CM36">
         <v>1</v>
-      </c>
-      <c r="CN36">
-        <v>0</v>
       </c>
       <c r="CO36">
         <f t="shared" si="18"/>
-        <v>683.19747450200543</v>
+        <v>680.59456329988268</v>
       </c>
       <c r="CQ36">
         <v>33</v>
@@ -11296,7 +11192,7 @@
         <v>727.33174048783565</v>
       </c>
     </row>
-    <row r="37" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:101" s="2" customFormat="1">
       <c r="A37">
         <v>34</v>
       </c>
@@ -11545,29 +11441,27 @@
         <v>34</v>
       </c>
       <c r="CH37">
-        <v>1170.5599847538599</v>
+        <v>1171.7127333449</v>
       </c>
       <c r="CI37">
-        <v>2.44360877070742E-2</v>
+        <v>2.7176396238686999E-2</v>
       </c>
       <c r="CJ37">
-        <v>0.23692769184595799</v>
+        <v>0.27656065885600101</v>
       </c>
       <c r="CK37">
         <v>1</v>
       </c>
       <c r="CL37">
-        <v>3.1644501632790301E-3</v>
+        <v>3.3387060516981201E-3</v>
       </c>
       <c r="CM37">
-        <v>0.80487233891559296</v>
-      </c>
-      <c r="CN37">
-        <v>4.3473532485477197E-3</v>
-      </c>
+        <v>4.1238649635631702E-2</v>
+      </c>
+      <c r="CN37"/>
       <c r="CO37">
         <f t="shared" si="18"/>
-        <v>1183.1731234399913</v>
+        <v>1182.1475159535958</v>
       </c>
       <c r="CQ37">
         <v>34</v>
@@ -11592,7 +11486,7 @@
         <v>1302.9224860259728</v>
       </c>
     </row>
-    <row r="38" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:101">
       <c r="A38">
         <v>35</v>
       </c>
@@ -11687,11 +11581,11 @@
       </c>
       <c r="AF38">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG38">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH38">
         <f t="shared" si="11"/>
@@ -11840,29 +11734,26 @@
         <v>35</v>
       </c>
       <c r="CH38">
-        <v>740.34333473594199</v>
+        <v>744.75773122133603</v>
       </c>
       <c r="CI38">
-        <v>4.5185434380067599E-2</v>
+        <v>4.2855024978338499E-2</v>
       </c>
       <c r="CJ38">
-        <v>0.24770663154134601</v>
+        <v>0.24421460226442801</v>
       </c>
       <c r="CK38">
         <v>1</v>
       </c>
       <c r="CL38">
-        <v>6.8108542713621496E-3</v>
+        <v>9.0336028446582495E-3</v>
       </c>
       <c r="CM38">
-        <v>0.50983415191844506</v>
-      </c>
-      <c r="CN38">
-        <v>0</v>
+        <v>0.64727942040465203</v>
       </c>
       <c r="CO38">
         <f t="shared" si="18"/>
-        <v>752.95647342207337</v>
+        <v>755.19251383003166</v>
       </c>
       <c r="CQ38">
         <v>35</v>
@@ -11887,7 +11778,7 @@
         <v>791.79762071087657</v>
       </c>
     </row>
-    <row r="39" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:101">
       <c r="F39">
         <f>AVERAGE(F3:F38)</f>
         <v>7.4534027524388686E-3</v>
@@ -11906,7 +11797,7 @@
       </c>
       <c r="AA39">
         <f>SUM(AA3:AA38)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="AB39">
         <f t="shared" ref="AB39:AH39" si="20">SUM(AB3:AB38)</f>
@@ -11914,7 +11805,7 @@
       </c>
       <c r="AC39">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD39">
         <f t="shared" si="20"/>
@@ -11922,15 +11813,15 @@
       </c>
       <c r="AE39">
         <f t="shared" si="20"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AF39">
         <f t="shared" si="20"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AG39">
         <f t="shared" si="20"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AH39">
         <f t="shared" si="20"/>
@@ -11958,14 +11849,14 @@
       </c>
       <c r="CO39">
         <f>SUM(CO3:CO38)</f>
-        <v>38350.774126374112</v>
+        <v>38258.422408013372</v>
       </c>
       <c r="CW39">
         <f>SUM(CW3:CW38)</f>
         <v>40507.282365096406</v>
       </c>
     </row>
-    <row r="40" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:101">
       <c r="A40" t="s">
         <v>8</v>
       </c>

</xml_diff>